<commit_message>
RNN and SVM SGD models finalised
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB4BAF30-76AF-4A7B-9AD6-3ABD88FB1A3B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94637345-F8DC-47B4-96B9-3E4709654C9F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="42">
   <si>
     <t>Low</t>
   </si>
@@ -109,13 +109,61 @@
   </si>
   <si>
     <t>Model Summaries</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>ROC AUC</t>
+  </si>
+  <si>
+    <t>PR AUC</t>
+  </si>
+  <si>
+    <t>Earthquake Train</t>
+  </si>
+  <si>
+    <t>Flood - Train</t>
+  </si>
+  <si>
+    <t>Earthquake - Test</t>
+  </si>
+  <si>
+    <t>Flood - Test</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>1. SVM SGD (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. SVM SGD (Med Vs Critical)</t>
+  </si>
+  <si>
+    <t>For all the following I used the Earthquake and Flood data from 2018 (train and test combined). Training was done on 80% of the data and validation on the remaining 20%.</t>
+  </si>
+  <si>
+    <t>3. SVM SGD (High Vs Crit)</t>
+  </si>
+  <si>
+    <t>1. RNN LSTM (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. RNN LSTM (Medium Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. RNN LSTM (High Vs Critical)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +213,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -204,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -333,11 +417,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -403,6 +513,38 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,17 +859,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
-  <dimension ref="B2:Z28"/>
+  <dimension ref="B2:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" customWidth="1"/>
     <col min="11" max="11" width="15.08984375" customWidth="1"/>
+    <col min="14" max="14" width="13.7265625" customWidth="1"/>
     <col min="20" max="20" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -881,25 +1026,25 @@
       <c r="H7" s="6">
         <v>1333</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="30">
         <v>205</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="30">
         <v>22</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="30">
         <v>19</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="31">
         <v>1</v>
       </c>
-      <c r="P7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4">
+      <c r="P7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="30">
         <f t="shared" ref="Q7:Q10" si="0">SUM(L7:P7)</f>
         <v>247</v>
       </c>
@@ -1021,25 +1166,25 @@
         <f>SUM(C9:G9)</f>
         <v>7984</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="30">
         <v>107</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="30">
         <v>69</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="30">
         <v>56</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="31">
         <v>3</v>
       </c>
-      <c r="P9" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4">
+      <c r="P9" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="30">
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
@@ -1245,25 +1390,25 @@
       </c>
     </row>
     <row r="15" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="30">
         <v>3499</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="30">
         <v>740</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="30">
         <v>630</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="6">
         <v>24</v>
       </c>
-      <c r="P15" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="4">
+      <c r="P15" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="30">
         <f>SUM(L15:P15)</f>
         <v>4893</v>
       </c>
@@ -1341,25 +1486,25 @@
       </c>
     </row>
     <row r="17" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="30">
         <v>1659</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="30">
         <v>305</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="30">
         <v>292</v>
       </c>
-      <c r="O17" s="13">
+      <c r="O17" s="6">
         <v>27</v>
       </c>
-      <c r="P17" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="4">
+      <c r="P17" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="30">
         <f t="shared" si="2"/>
         <v>2283</v>
       </c>
@@ -1612,6 +1757,435 @@
         <v>25</v>
       </c>
     </row>
+    <row r="30" spans="2:26" ht="21" x14ac:dyDescent="0.5">
+      <c r="B30" s="32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="D32" s="38"/>
+      <c r="E32" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D33" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="33">
+        <v>205</v>
+      </c>
+      <c r="F33" s="33">
+        <v>22</v>
+      </c>
+      <c r="G33" s="33">
+        <v>19</v>
+      </c>
+      <c r="H33" s="36">
+        <v>1</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <f>SUM(E33:I33)</f>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D34" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="33">
+        <v>107</v>
+      </c>
+      <c r="F34" s="33">
+        <v>69</v>
+      </c>
+      <c r="G34" s="33">
+        <v>56</v>
+      </c>
+      <c r="H34" s="36">
+        <v>3</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <f>SUM(E34:I34)</f>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D35" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="33">
+        <v>3499</v>
+      </c>
+      <c r="F35" s="33">
+        <v>740</v>
+      </c>
+      <c r="G35" s="33">
+        <v>630</v>
+      </c>
+      <c r="H35" s="37">
+        <v>24</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <f>SUM(E35:I35)</f>
+        <v>4893</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D36" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="33">
+        <v>1659</v>
+      </c>
+      <c r="F36" s="33">
+        <v>305</v>
+      </c>
+      <c r="G36" s="33">
+        <v>292</v>
+      </c>
+      <c r="H36" s="37">
+        <v>27</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <f>SUM(E36:I36)</f>
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="J37" s="39">
+        <f>SUM(J33:J36)</f>
+        <v>7658</v>
+      </c>
+    </row>
+    <row r="40" spans="3:16" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C40" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+    </row>
+    <row r="41" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+    </row>
+    <row r="42" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C42" s="16"/>
+      <c r="D42" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="40">
+        <v>55</v>
+      </c>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" s="16"/>
+      <c r="I42" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="J42" s="40">
+        <v>55</v>
+      </c>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="O42" s="40">
+        <v>55</v>
+      </c>
+      <c r="P42" s="16"/>
+    </row>
+    <row r="43" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C43" s="16"/>
+      <c r="D43" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="40">
+        <v>200</v>
+      </c>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="J43" s="40">
+        <v>200</v>
+      </c>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="O43" s="40">
+        <v>200</v>
+      </c>
+      <c r="P43" s="16"/>
+    </row>
+    <row r="44" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C44" s="16"/>
+      <c r="D44" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="41">
+        <v>0.182</v>
+      </c>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" s="41">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="O44" s="41">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="P44" s="16"/>
+    </row>
+    <row r="45" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C45" s="16"/>
+      <c r="D45" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="41">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="J45" s="41">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="O45" s="41">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="P45" s="16"/>
+    </row>
+    <row r="46" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C46" s="16"/>
+      <c r="D46" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="40">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="J46" s="40">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="O46" s="40">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="P46" s="16"/>
+    </row>
+    <row r="47" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C47" s="16"/>
+      <c r="D47" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="40">
+        <v>0.54</v>
+      </c>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" s="40">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="O47" s="40">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="P47" s="16"/>
+    </row>
+    <row r="54" spans="3:15" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C54" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="H54" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="M54" s="42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="3:15" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D56" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="40">
+        <v>55</v>
+      </c>
+      <c r="I56" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56" s="40">
+        <v>55</v>
+      </c>
+      <c r="N56" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="O56" s="40">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D57" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="40">
+        <v>200</v>
+      </c>
+      <c r="I57" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="J57" s="40">
+        <v>200</v>
+      </c>
+      <c r="N57" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="O57" s="40">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="3:15" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D58" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="41">
+        <v>1</v>
+      </c>
+      <c r="I58" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J58" s="41">
+        <v>1</v>
+      </c>
+      <c r="N58" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="O58" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="3:15" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D59" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="41">
+        <v>0.249</v>
+      </c>
+      <c r="I59" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="J59" s="41">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="N59" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="O59" s="41">
+        <v>0.1948</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tfidf corrected and initial word emnedding own
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7E6E64-6984-46E9-896B-507E40596B29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB853D3-B4FA-4B12-8B1D-0921E1FDCBBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
+    <workbookView xWindow="3640" yWindow="3640" windowWidth="13220" windowHeight="10990" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
   <si>
     <t>Low</t>
   </si>
@@ -117,12 +117,6 @@
     <t>Precision</t>
   </si>
   <si>
-    <t>ROC AUC</t>
-  </si>
-  <si>
-    <t>PR AUC</t>
-  </si>
-  <si>
     <t>Earthquake Train</t>
   </si>
   <si>
@@ -232,6 +226,21 @@
   </si>
   <si>
     <t>Fit:</t>
+  </si>
+  <si>
+    <t>Mean Precision</t>
+  </si>
+  <si>
+    <t>Mean Recall</t>
+  </si>
+  <si>
+    <t>Mean ROC AUC</t>
+  </si>
+  <si>
+    <t>Mean PR AUC</t>
+  </si>
+  <si>
+    <t>SD</t>
   </si>
 </sst>
 </file>
@@ -303,13 +312,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -325,9 +327,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <i/>
+      <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -377,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -545,11 +554,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -624,7 +713,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -644,8 +732,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -654,10 +742,22 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
   <dimension ref="B2:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,9 +1083,9 @@
     <col min="2" max="2" width="14.6328125" customWidth="1"/>
     <col min="4" max="4" width="19.453125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.08984375" customWidth="1"/>
     <col min="11" max="11" width="15.08984375" customWidth="1"/>
-    <col min="14" max="14" width="13.7265625" customWidth="1"/>
+    <col min="14" max="14" width="17.81640625" customWidth="1"/>
     <col min="20" max="20" width="29.6328125" customWidth="1"/>
     <col min="21" max="21" width="21.81640625" customWidth="1"/>
     <col min="23" max="23" width="21.08984375" customWidth="1"/>
@@ -1854,7 +1954,10 @@
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
-      <c r="O23" s="21"/>
+      <c r="O23" s="21">
+        <f>SUM(O15:O22)</f>
+        <v>129</v>
+      </c>
       <c r="P23" s="21"/>
       <c r="Q23" s="22">
         <f>SUM(Q15:Q22)</f>
@@ -1875,553 +1978,788 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:26" ht="21" x14ac:dyDescent="0.5">
-      <c r="B30" s="32" t="s">
-        <v>36</v>
-      </c>
+    <row r="30" spans="2:26" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B30" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="58"/>
+      <c r="S30" s="59"/>
+      <c r="T30" s="60"/>
+    </row>
+    <row r="31" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B31" s="53"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="52"/>
     </row>
     <row r="32" spans="2:26" ht="29" x14ac:dyDescent="0.35">
-      <c r="D32" s="38"/>
-      <c r="E32" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" s="35" t="s">
+      <c r="B32" s="53"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="H32" s="34" t="s">
+      <c r="H32" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="35" t="s">
+      <c r="I32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="J32" s="35" t="s">
+      <c r="J32" s="34" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="D33" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="33">
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="52"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B33" s="53"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="32">
         <v>205</v>
       </c>
-      <c r="F33" s="33">
+      <c r="F33" s="32">
         <v>22</v>
       </c>
-      <c r="G33" s="33">
+      <c r="G33" s="32">
         <v>19</v>
       </c>
-      <c r="H33" s="36">
+      <c r="H33" s="35">
         <v>1</v>
       </c>
-      <c r="I33" s="33">
-        <v>0</v>
-      </c>
-      <c r="J33" s="33">
+      <c r="I33" s="32">
+        <v>0</v>
+      </c>
+      <c r="J33" s="32">
         <f>SUM(E33:I33)</f>
         <v>247</v>
       </c>
-    </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="D34" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="33">
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="52"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B34" s="53"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="32">
         <v>107</v>
       </c>
-      <c r="F34" s="33">
+      <c r="F34" s="32">
         <v>69</v>
       </c>
-      <c r="G34" s="33">
+      <c r="G34" s="32">
         <v>56</v>
       </c>
-      <c r="H34" s="36">
+      <c r="H34" s="35">
         <v>3</v>
       </c>
-      <c r="I34" s="33">
-        <v>0</v>
-      </c>
-      <c r="J34" s="33">
+      <c r="I34" s="32">
+        <v>0</v>
+      </c>
+      <c r="J34" s="32">
         <f>SUM(E34:I34)</f>
         <v>235</v>
       </c>
-    </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="D35" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="33">
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="52"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B35" s="53"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="32">
         <v>3499</v>
       </c>
-      <c r="F35" s="33">
+      <c r="F35" s="32">
         <v>740</v>
       </c>
-      <c r="G35" s="33">
+      <c r="G35" s="32">
         <v>630</v>
       </c>
-      <c r="H35" s="37">
+      <c r="H35" s="36">
         <v>24</v>
       </c>
-      <c r="I35" s="33">
-        <v>0</v>
-      </c>
-      <c r="J35" s="33">
+      <c r="I35" s="32">
+        <v>0</v>
+      </c>
+      <c r="J35" s="32">
         <f>SUM(E35:I35)</f>
         <v>4893</v>
       </c>
-    </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="D36" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="33">
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="52"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B36" s="53"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="32">
         <v>1659</v>
       </c>
-      <c r="F36" s="33">
+      <c r="F36" s="32">
         <v>305</v>
       </c>
-      <c r="G36" s="33">
+      <c r="G36" s="32">
         <v>292</v>
       </c>
-      <c r="H36" s="37">
+      <c r="H36" s="36">
         <v>27</v>
       </c>
-      <c r="I36" s="33">
-        <v>0</v>
-      </c>
-      <c r="J36" s="33">
+      <c r="I36" s="32">
+        <v>0</v>
+      </c>
+      <c r="J36" s="32">
         <f>SUM(E36:I36)</f>
         <v>2283</v>
       </c>
-    </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="J37" s="39">
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="52"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B37" s="53"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16">
+        <f>SUM(H33:H36)</f>
+        <v>55</v>
+      </c>
+      <c r="I37" s="16"/>
+      <c r="J37" s="38">
         <f>SUM(J33:J36)</f>
         <v>7658</v>
       </c>
-    </row>
-    <row r="40" spans="3:16" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C40" s="42" t="s">
-        <v>34</v>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="52"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B38" s="53"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="52"/>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B39" s="53"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="52"/>
+    </row>
+    <row r="40" spans="2:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="53"/>
+      <c r="C40" s="41" t="s">
+        <v>32</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
-      <c r="H40" s="42" t="s">
-        <v>35</v>
+      <c r="H40" s="41" t="s">
+        <v>33</v>
       </c>
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
-      <c r="M40" s="42" t="s">
-        <v>37</v>
+      <c r="M40" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
       <c r="P40" s="16"/>
-    </row>
-    <row r="41" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="52"/>
+    </row>
+    <row r="41" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B41" s="53"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
+      <c r="F41" s="51" t="s">
+        <v>69</v>
+      </c>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
+      <c r="K41" s="51" t="s">
+        <v>69</v>
+      </c>
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
-      <c r="P41" s="16"/>
-    </row>
-    <row r="42" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="P41" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="52"/>
+    </row>
+    <row r="42" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B42" s="53"/>
       <c r="C42" s="16"/>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="40">
+      <c r="E42" s="39">
         <v>55</v>
       </c>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
-      <c r="I42" s="40" t="s">
+      <c r="I42" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="J42" s="40">
+      <c r="J42" s="39">
         <v>55</v>
       </c>
       <c r="K42" s="16"/>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
-      <c r="N42" s="40" t="s">
+      <c r="N42" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="O42" s="40">
+      <c r="O42" s="39">
         <v>55</v>
       </c>
       <c r="P42" s="16"/>
-    </row>
-    <row r="43" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="52"/>
+    </row>
+    <row r="43" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B43" s="53"/>
       <c r="C43" s="16"/>
-      <c r="D43" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="40">
-        <v>200</v>
+      <c r="D43" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="39">
+        <v>55</v>
       </c>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
-      <c r="I43" s="40" t="s">
+      <c r="I43" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="J43" s="40">
-        <v>200</v>
+      <c r="J43" s="39">
+        <v>55</v>
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
-      <c r="N43" s="40" t="s">
+      <c r="N43" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="O43" s="40">
-        <v>200</v>
+      <c r="O43" s="39">
+        <v>55</v>
       </c>
       <c r="P43" s="16"/>
-    </row>
-    <row r="44" spans="3:16" ht="21" x14ac:dyDescent="0.5">
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="52"/>
+    </row>
+    <row r="44" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B44" s="53"/>
       <c r="C44" s="16"/>
-      <c r="D44" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="E44" s="41">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="F44" s="16"/>
+      <c r="D44" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" s="40">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="F44" s="49">
+        <v>0.22800000000000001</v>
+      </c>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
-      <c r="I44" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="J44" s="51">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="K44" s="16"/>
+      <c r="I44" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" s="40">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="K44" s="49">
+        <v>0.2</v>
+      </c>
       <c r="L44" s="16"/>
       <c r="M44" s="16"/>
-      <c r="N44" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="O44" s="41">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="P44" s="16"/>
-    </row>
-    <row r="45" spans="3:16" ht="21" x14ac:dyDescent="0.5">
+      <c r="N44" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="O44" s="40">
+        <v>0.499</v>
+      </c>
+      <c r="P44" s="49">
+        <v>0.217</v>
+      </c>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="52"/>
+    </row>
+    <row r="45" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B45" s="53"/>
       <c r="C45" s="16"/>
-      <c r="D45" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="41">
-        <v>1</v>
-      </c>
-      <c r="F45" s="16"/>
+      <c r="D45" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" s="40">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="F45" s="49">
+        <v>0.18099999999999999</v>
+      </c>
       <c r="G45" s="16"/>
       <c r="H45" s="16"/>
-      <c r="I45" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="J45" s="51">
-        <v>0.6</v>
-      </c>
-      <c r="K45" s="16"/>
+      <c r="I45" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="J45" s="40">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="K45" s="49">
+        <v>0.16300000000000001</v>
+      </c>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
-      <c r="N45" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="O45" s="41">
-        <v>1</v>
-      </c>
-      <c r="P45" s="16"/>
-    </row>
-    <row r="46" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="N45" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="O45" s="40">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="P45" s="49">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="52"/>
+    </row>
+    <row r="46" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B46" s="53"/>
       <c r="C46" s="16"/>
-      <c r="D46" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="E46" s="40">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="F46" s="16"/>
+      <c r="D46" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="39">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="F46" s="49">
+        <v>0.104</v>
+      </c>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
-      <c r="I46" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="J46" s="40">
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="K46" s="16"/>
+      <c r="I46" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="J46" s="39">
+        <v>0.745</v>
+      </c>
+      <c r="K46" s="49">
+        <v>0.06</v>
+      </c>
       <c r="L46" s="16"/>
       <c r="M46" s="16"/>
-      <c r="N46" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="O46" s="40">
-        <v>0.74</v>
-      </c>
-      <c r="P46" s="16"/>
-    </row>
-    <row r="47" spans="3:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="N46" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="O46" s="39">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="P46" s="49">
+        <v>7.8E-2</v>
+      </c>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="52"/>
+    </row>
+    <row r="47" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B47" s="53"/>
       <c r="C47" s="16"/>
-      <c r="D47" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E47" s="50">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="F47" s="49"/>
+      <c r="D47" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" s="48">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="F47" s="50">
+        <v>0.123</v>
+      </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
-      <c r="I47" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="J47" s="50">
-        <v>0.46800000000000003</v>
-      </c>
-      <c r="K47" s="49"/>
+      <c r="I47" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="J47" s="48">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="K47" s="50">
+        <v>5.5E-2</v>
+      </c>
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
-      <c r="N47" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="O47" s="50">
-        <v>0.48899999999999999</v>
-      </c>
-      <c r="P47" s="49"/>
+      <c r="N47" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="O47" s="48">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="P47" s="50">
+        <v>0.104</v>
+      </c>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="52"/>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B48" s="54"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="55"/>
+      <c r="M48" s="55"/>
+      <c r="N48" s="55"/>
+      <c r="O48" s="55"/>
+      <c r="P48" s="55"/>
+      <c r="Q48" s="55"/>
+      <c r="R48" s="55"/>
+      <c r="S48" s="56"/>
     </row>
     <row r="54" spans="3:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C54" s="42" t="s">
+      <c r="C54" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="H54" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="M54" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="H54" s="42" t="s">
+      <c r="T54" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="W54" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z54" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB54" s="47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="T55" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="M54" s="42" t="s">
+      <c r="U55" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="W55" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D56" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="39">
+        <v>55</v>
+      </c>
+      <c r="I56" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56" s="39">
+        <v>55</v>
+      </c>
+      <c r="N56" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O56" s="39">
+        <v>55</v>
+      </c>
+      <c r="T56" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="T54" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="W54" s="48" t="s">
+      <c r="U56" s="43">
+        <v>2</v>
+      </c>
+      <c r="W56" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="Z54" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB54" s="48" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="T55" s="44" t="s">
+      <c r="X56" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z56" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA56" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB56" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC56" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D57" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="39">
+        <v>200</v>
+      </c>
+      <c r="I57" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J57" s="39">
+        <v>200</v>
+      </c>
+      <c r="N57" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="O57" s="39">
+        <v>200</v>
+      </c>
+      <c r="T57" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="U55" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="W55" s="43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="D56" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="E56" s="40">
+      <c r="U57" s="43">
+        <v>1</v>
+      </c>
+      <c r="W57" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="X57" s="43">
+        <v>4</v>
+      </c>
+      <c r="Z57" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="I56" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="J56" s="40">
-        <v>55</v>
-      </c>
-      <c r="N56" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="O56" s="40">
-        <v>55</v>
-      </c>
-      <c r="T56" s="44" t="s">
+      <c r="AA57" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB57" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC57" s="43">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D58" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="40">
+        <v>1</v>
+      </c>
+      <c r="I58" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J58" s="40">
+        <v>1</v>
+      </c>
+      <c r="N58" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="O58" s="40">
+        <v>1</v>
+      </c>
+      <c r="T58" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="U56" s="44">
-        <v>2</v>
-      </c>
-      <c r="W56" s="44" t="s">
+      <c r="U58" s="43">
+        <v>1</v>
+      </c>
+      <c r="W58" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="X58" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="AB58" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC58" s="43">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="59" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D59" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="40">
+        <v>0.249</v>
+      </c>
+      <c r="I59" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="J59" s="40">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="N59" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="O59" s="40">
+        <v>0.1948</v>
+      </c>
+      <c r="AB59" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC59" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="W60" s="42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="W61" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="X61" s="44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="W62" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="X56" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z56" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA56" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB56" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC56" s="44">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="D57" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="40">
-        <v>200</v>
-      </c>
-      <c r="I57" s="40" t="s">
+      <c r="X62" s="43">
         <v>1</v>
       </c>
-      <c r="J57" s="40">
-        <v>200</v>
-      </c>
-      <c r="N57" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="O57" s="40">
-        <v>200</v>
-      </c>
-      <c r="T57" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="U57" s="44">
-        <v>1</v>
-      </c>
-      <c r="W57" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="X57" s="44">
-        <v>4</v>
-      </c>
-      <c r="Z57" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA57" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB57" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC57" s="44">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="D58" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="E58" s="41">
-        <v>1</v>
-      </c>
-      <c r="I58" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="J58" s="41">
-        <v>1</v>
-      </c>
-      <c r="N58" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="O58" s="41">
-        <v>1</v>
-      </c>
-      <c r="T58" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="U58" s="44">
-        <v>1</v>
-      </c>
-      <c r="W58" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="X58" s="46">
-        <v>0.2</v>
-      </c>
-      <c r="AB58" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC58" s="44">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="59" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="D59" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E59" s="41">
-        <v>0.249</v>
-      </c>
-      <c r="I59" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="J59" s="41">
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="N59" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="O59" s="41">
-        <v>0.1948</v>
-      </c>
-      <c r="AB59" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC59" s="44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="W60" s="43" t="s">
+    </row>
+    <row r="63" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="W63" s="43" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="61" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="W61" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="X61" s="45" t="s">
+      <c r="X63" s="44" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="62" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="W62" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="X62" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="W63" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="X63" s="45" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
word embedding LSTM complete
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB853D3-B4FA-4B12-8B1D-0921E1FDCBBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312225C7-B67E-4FEB-8BC9-31B35D96E3BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="3640" windowWidth="13220" windowHeight="10990" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="76">
   <si>
     <t>Low</t>
   </si>
@@ -141,15 +141,6 @@
     <t>3. SVM SGD (High Vs Crit)</t>
   </si>
   <si>
-    <t>1. RNN LSTM (Low Vs Critical)</t>
-  </si>
-  <si>
-    <t>2. RNN LSTM (Medium Vs Critical)</t>
-  </si>
-  <si>
-    <t>3. RNN LSTM (High Vs Critical)</t>
-  </si>
-  <si>
     <t>Model Type</t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>Model Parameters:</t>
   </si>
   <si>
-    <t>RNN using LSTM</t>
-  </si>
-  <si>
     <t>Layer Parameters:</t>
   </si>
   <si>
@@ -195,9 +183,6 @@
     <t>Activation</t>
   </si>
   <si>
-    <t>Softmax</t>
-  </si>
-  <si>
     <t>Optimizer</t>
   </si>
   <si>
@@ -241,6 +226,39 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>1. RNN LSTM TFIDF (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. RNN LSTM TFIDF (Medium Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. RNN LSTM TFIDF (High Vs Critical)</t>
+  </si>
+  <si>
+    <t>1. RNN LSTM Embeddings (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. RNN LSTM Embeddings (Med Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. RNN LSTM Embeddings (High Vs Critical)</t>
+  </si>
+  <si>
+    <t>RNN using LSTM &amp; TFIDF</t>
+  </si>
+  <si>
+    <t>RNN using LSTM &amp; Embedding</t>
+  </si>
+  <si>
+    <t>Embedding</t>
+  </si>
+  <si>
+    <t>Dimension/Word</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
   </si>
 </sst>
 </file>
@@ -386,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -634,11 +652,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -735,14 +768,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -758,6 +789,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
-  <dimension ref="B2:AC63"/>
+  <dimension ref="B2:AD80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N49" sqref="N49"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="52" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1087,8 +1130,9 @@
     <col min="11" max="11" width="15.08984375" customWidth="1"/>
     <col min="14" max="14" width="17.81640625" customWidth="1"/>
     <col min="20" max="20" width="29.6328125" customWidth="1"/>
-    <col min="21" max="21" width="21.81640625" customWidth="1"/>
+    <col min="21" max="21" width="29.1796875" customWidth="1"/>
     <col min="23" max="23" width="21.08984375" customWidth="1"/>
+    <col min="24" max="24" width="15.1796875" customWidth="1"/>
     <col min="26" max="26" width="14.26953125" customWidth="1"/>
     <col min="27" max="27" width="21" customWidth="1"/>
     <col min="28" max="28" width="11.81640625" customWidth="1"/>
@@ -1979,30 +2023,30 @@
       </c>
     </row>
     <row r="30" spans="2:26" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="59"/>
-      <c r="T30" s="60"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="56"/>
+      <c r="S30" s="57"/>
+      <c r="T30" s="58"/>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="B31" s="53"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -2019,10 +2063,10 @@
       <c r="P31" s="16"/>
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
-      <c r="S31" s="52"/>
+      <c r="S31" s="50"/>
     </row>
     <row r="32" spans="2:26" ht="29" x14ac:dyDescent="0.35">
-      <c r="B32" s="53"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="16"/>
       <c r="D32" s="37"/>
       <c r="E32" s="34" t="s">
@@ -2051,10 +2095,10 @@
       <c r="P32" s="16"/>
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
-      <c r="S32" s="52"/>
+      <c r="S32" s="50"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B33" s="53"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="16"/>
       <c r="D33" s="32" t="s">
         <v>28</v>
@@ -2086,10 +2130,10 @@
       <c r="P33" s="16"/>
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
-      <c r="S33" s="52"/>
+      <c r="S33" s="50"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B34" s="53"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="16"/>
       <c r="D34" s="32" t="s">
         <v>29</v>
@@ -2121,10 +2165,10 @@
       <c r="P34" s="16"/>
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
-      <c r="S34" s="52"/>
+      <c r="S34" s="50"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B35" s="53"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="16"/>
       <c r="D35" s="32" t="s">
         <v>30</v>
@@ -2156,10 +2200,10 @@
       <c r="P35" s="16"/>
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
-      <c r="S35" s="52"/>
+      <c r="S35" s="50"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B36" s="53"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="16"/>
       <c r="D36" s="32" t="s">
         <v>31</v>
@@ -2191,10 +2235,10 @@
       <c r="P36" s="16"/>
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
-      <c r="S36" s="52"/>
+      <c r="S36" s="50"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B37" s="53"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -2217,10 +2261,10 @@
       <c r="P37" s="16"/>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
-      <c r="S37" s="52"/>
+      <c r="S37" s="50"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B38" s="53"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -2237,10 +2281,10 @@
       <c r="P38" s="16"/>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
-      <c r="S38" s="52"/>
+      <c r="S38" s="50"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B39" s="53"/>
+      <c r="B39" s="51"/>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2257,10 +2301,10 @@
       <c r="P39" s="16"/>
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
-      <c r="S39" s="52"/>
+      <c r="S39" s="50"/>
     </row>
     <row r="40" spans="2:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="53"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="41" t="s">
         <v>32</v>
       </c>
@@ -2283,36 +2327,36 @@
       <c r="P40" s="16"/>
       <c r="Q40" s="16"/>
       <c r="R40" s="16"/>
-      <c r="S40" s="52"/>
+      <c r="S40" s="50"/>
     </row>
     <row r="41" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B41" s="53"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
-      <c r="F41" s="51" t="s">
-        <v>69</v>
+      <c r="F41" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
-      <c r="K41" s="51" t="s">
-        <v>69</v>
+      <c r="K41" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
-      <c r="P41" s="51" t="s">
-        <v>69</v>
+      <c r="P41" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
-      <c r="S41" s="52"/>
+      <c r="S41" s="50"/>
     </row>
     <row r="42" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B42" s="53"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="16"/>
       <c r="D42" s="39" t="s">
         <v>3</v>
@@ -2341,10 +2385,10 @@
       <c r="P42" s="16"/>
       <c r="Q42" s="16"/>
       <c r="R42" s="16"/>
-      <c r="S42" s="52"/>
+      <c r="S42" s="50"/>
     </row>
     <row r="43" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B43" s="53"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="16"/>
       <c r="D43" s="39" t="s">
         <v>0</v>
@@ -2373,394 +2417,1285 @@
       <c r="P43" s="16"/>
       <c r="Q43" s="16"/>
       <c r="R43" s="16"/>
-      <c r="S43" s="52"/>
+      <c r="S43" s="50"/>
     </row>
     <row r="44" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B44" s="53"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="16"/>
       <c r="D44" s="40" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E44" s="40">
         <v>0.70299999999999996</v>
       </c>
-      <c r="F44" s="49">
+      <c r="F44" s="47">
         <v>0.22800000000000001</v>
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
       <c r="I44" s="40" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J44" s="40">
         <v>0.59599999999999997</v>
       </c>
-      <c r="K44" s="49">
+      <c r="K44" s="47">
         <v>0.2</v>
       </c>
       <c r="L44" s="16"/>
       <c r="M44" s="16"/>
       <c r="N44" s="40" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="O44" s="40">
         <v>0.499</v>
       </c>
-      <c r="P44" s="49">
+      <c r="P44" s="47">
         <v>0.217</v>
       </c>
       <c r="Q44" s="16"/>
       <c r="R44" s="16"/>
-      <c r="S44" s="52"/>
+      <c r="S44" s="50"/>
     </row>
     <row r="45" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B45" s="53"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="16"/>
       <c r="D45" s="40" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E45" s="40">
         <v>0.80500000000000005</v>
       </c>
-      <c r="F45" s="49">
+      <c r="F45" s="47">
         <v>0.18099999999999999</v>
       </c>
       <c r="G45" s="16"/>
       <c r="H45" s="16"/>
       <c r="I45" s="40" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J45" s="40">
         <v>0.74299999999999999</v>
       </c>
-      <c r="K45" s="49">
+      <c r="K45" s="47">
         <v>0.16300000000000001</v>
       </c>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
       <c r="N45" s="40" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O45" s="40">
         <v>0.66700000000000004</v>
       </c>
-      <c r="P45" s="49">
+      <c r="P45" s="47">
         <v>0.16200000000000001</v>
       </c>
       <c r="Q45" s="16"/>
       <c r="R45" s="16"/>
-      <c r="S45" s="52"/>
+      <c r="S45" s="50"/>
     </row>
     <row r="46" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B46" s="53"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="16"/>
       <c r="D46" s="39" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E46" s="39">
         <v>0.81599999999999995</v>
       </c>
-      <c r="F46" s="49">
+      <c r="F46" s="47">
         <v>0.104</v>
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
       <c r="I46" s="39" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J46" s="39">
         <v>0.745</v>
       </c>
-      <c r="K46" s="49">
+      <c r="K46" s="47">
         <v>0.06</v>
       </c>
       <c r="L46" s="16"/>
       <c r="M46" s="16"/>
       <c r="N46" s="39" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O46" s="39">
         <v>0.71199999999999997</v>
       </c>
-      <c r="P46" s="49">
+      <c r="P46" s="47">
         <v>7.8E-2</v>
       </c>
       <c r="Q46" s="16"/>
       <c r="R46" s="16"/>
-      <c r="S46" s="52"/>
+      <c r="S46" s="50"/>
     </row>
     <row r="47" spans="2:19" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B47" s="53"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="16"/>
       <c r="D47" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E47" s="48">
+        <v>63</v>
+      </c>
+      <c r="E47" s="46">
         <v>0.82399999999999995</v>
       </c>
-      <c r="F47" s="50">
+      <c r="F47" s="48">
         <v>0.123</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
       <c r="I47" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J47" s="48">
+        <v>63</v>
+      </c>
+      <c r="J47" s="46">
         <v>0.80600000000000005</v>
       </c>
-      <c r="K47" s="50">
+      <c r="K47" s="48">
         <v>5.5E-2</v>
       </c>
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
       <c r="N47" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="O47" s="48">
+        <v>63</v>
+      </c>
+      <c r="O47" s="46">
         <v>0.73399999999999999</v>
       </c>
-      <c r="P47" s="50">
+      <c r="P47" s="48">
         <v>0.104</v>
       </c>
       <c r="Q47" s="16"/>
       <c r="R47" s="16"/>
-      <c r="S47" s="52"/>
+      <c r="S47" s="50"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B48" s="54"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="55"/>
-      <c r="N48" s="55"/>
-      <c r="O48" s="55"/>
-      <c r="P48" s="55"/>
-      <c r="Q48" s="55"/>
-      <c r="R48" s="55"/>
-      <c r="S48" s="56"/>
-    </row>
-    <row r="54" spans="3:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C54" s="41" t="s">
+      <c r="B48" s="52"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="54"/>
+    </row>
+    <row r="53" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C53" s="65"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="62"/>
+      <c r="M53" s="62"/>
+      <c r="N53" s="62"/>
+      <c r="O53" s="62"/>
+      <c r="P53" s="62"/>
+      <c r="Q53" s="62"/>
+      <c r="R53" s="62"/>
+      <c r="S53" s="62"/>
+      <c r="T53" s="62"/>
+      <c r="U53" s="62"/>
+      <c r="V53" s="62"/>
+      <c r="W53" s="62"/>
+      <c r="X53" s="62"/>
+      <c r="Y53" s="62"/>
+      <c r="Z53" s="62"/>
+      <c r="AA53" s="62"/>
+      <c r="AB53" s="62"/>
+      <c r="AC53" s="62"/>
+      <c r="AD53" s="64"/>
+    </row>
+    <row r="54" spans="3:30" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C54" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+      <c r="T54" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="U54" s="16"/>
+      <c r="V54" s="16"/>
+      <c r="W54" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="X54" s="16"/>
+      <c r="Y54" s="16"/>
+      <c r="Z54" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA54" s="16"/>
+      <c r="AB54" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC54" s="16"/>
+      <c r="AD54" s="50"/>
+    </row>
+    <row r="55" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C55" s="51"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+      <c r="T55" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="H54" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="M54" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="T54" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="W54" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z54" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB54" s="47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="T55" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="U55" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="W55" s="42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="U55" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="V55" s="16"/>
+      <c r="W55" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="X55" s="16"/>
+      <c r="Y55" s="16"/>
+      <c r="Z55" s="16"/>
+      <c r="AA55" s="16"/>
+      <c r="AB55" s="16"/>
+      <c r="AC55" s="16"/>
+      <c r="AD55" s="50"/>
+    </row>
+    <row r="56" spans="3:30" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C56" s="51"/>
       <c r="D56" s="39" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="39">
         <v>55</v>
       </c>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
       <c r="I56" s="39" t="s">
         <v>3</v>
       </c>
       <c r="J56" s="39">
         <v>55</v>
       </c>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
       <c r="N56" s="39" t="s">
         <v>3</v>
       </c>
       <c r="O56" s="39">
         <v>55</v>
       </c>
-      <c r="T56" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="U56" s="43">
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
+      <c r="T56" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="U56" s="42">
         <v>2</v>
       </c>
-      <c r="W56" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="X56" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z56" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA56" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB56" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC56" s="43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="V56" s="16"/>
+      <c r="W56" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="X56" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y56" s="16"/>
+      <c r="Z56" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA56" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB56" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC56" s="42">
+        <v>15</v>
+      </c>
+      <c r="AD56" s="50"/>
+    </row>
+    <row r="57" spans="3:30" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C57" s="51"/>
       <c r="D57" s="39" t="s">
         <v>0</v>
       </c>
       <c r="E57" s="39">
         <v>200</v>
       </c>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
       <c r="I57" s="39" t="s">
         <v>1</v>
       </c>
       <c r="J57" s="39">
         <v>200</v>
       </c>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
       <c r="N57" s="39" t="s">
         <v>2</v>
       </c>
       <c r="O57" s="39">
         <v>200</v>
       </c>
-      <c r="T57" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="U57" s="43">
+      <c r="P57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="16"/>
+      <c r="S57" s="16"/>
+      <c r="T57" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="U57" s="42">
         <v>1</v>
       </c>
-      <c r="W57" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="X57" s="43">
-        <v>4</v>
-      </c>
-      <c r="Z57" s="43" t="s">
+      <c r="V57" s="16"/>
+      <c r="W57" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="X57" s="42">
+        <v>8</v>
+      </c>
+      <c r="Y57" s="16"/>
+      <c r="Z57" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA57" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB57" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="AA57" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB57" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC57" s="43">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="AC57" s="42">
+        <v>16</v>
+      </c>
+      <c r="AD57" s="50"/>
+    </row>
+    <row r="58" spans="3:30" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C58" s="51"/>
       <c r="D58" s="40" t="s">
         <v>26</v>
       </c>
       <c r="E58" s="40">
         <v>1</v>
       </c>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
       <c r="I58" s="40" t="s">
         <v>26</v>
       </c>
       <c r="J58" s="40">
         <v>1</v>
       </c>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
+      <c r="M58" s="16"/>
       <c r="N58" s="40" t="s">
         <v>26</v>
       </c>
       <c r="O58" s="40">
         <v>1</v>
       </c>
-      <c r="T58" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="U58" s="43">
+      <c r="P58" s="16"/>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
+      <c r="T58" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="U58" s="42">
         <v>1</v>
       </c>
-      <c r="W58" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="X58" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="AB58" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC58" s="43">
+      <c r="V58" s="16"/>
+      <c r="W58" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="X58" s="44">
+        <v>0.4</v>
+      </c>
+      <c r="Y58" s="16"/>
+      <c r="Z58" s="16"/>
+      <c r="AA58" s="16"/>
+      <c r="AB58" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC58" s="42">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="59" spans="3:29" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="AD58" s="50"/>
+    </row>
+    <row r="59" spans="3:30" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C59" s="51"/>
       <c r="D59" s="40" t="s">
         <v>27</v>
       </c>
       <c r="E59" s="40">
         <v>0.249</v>
       </c>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
       <c r="I59" s="40" t="s">
         <v>27</v>
       </c>
       <c r="J59" s="40">
         <v>0.23400000000000001</v>
       </c>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
       <c r="N59" s="40" t="s">
         <v>27</v>
       </c>
       <c r="O59" s="40">
         <v>0.1948</v>
       </c>
-      <c r="AB59" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC59" s="43" t="b">
+      <c r="P59" s="16"/>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
+      <c r="T59" s="16"/>
+      <c r="U59" s="16"/>
+      <c r="V59" s="16"/>
+      <c r="W59" s="16"/>
+      <c r="X59" s="16"/>
+      <c r="Y59" s="16"/>
+      <c r="Z59" s="16"/>
+      <c r="AA59" s="16"/>
+      <c r="AB59" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC59" s="42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="W60" s="42" t="s">
+      <c r="AD59" s="50"/>
+    </row>
+    <row r="60" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C60" s="51"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16"/>
+      <c r="L60" s="16"/>
+      <c r="M60" s="16"/>
+      <c r="N60" s="16"/>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
+      <c r="Q60" s="16"/>
+      <c r="R60" s="16"/>
+      <c r="S60" s="16"/>
+      <c r="T60" s="16"/>
+      <c r="U60" s="16"/>
+      <c r="V60" s="16"/>
+      <c r="W60" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="X60" s="16"/>
+      <c r="Y60" s="16"/>
+      <c r="Z60" s="16"/>
+      <c r="AA60" s="16"/>
+      <c r="AB60" s="16"/>
+      <c r="AC60" s="16"/>
+      <c r="AD60" s="50"/>
+    </row>
+    <row r="61" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C61" s="51"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+      <c r="Q61" s="16"/>
+      <c r="R61" s="16"/>
+      <c r="S61" s="16"/>
+      <c r="T61" s="16"/>
+      <c r="U61" s="16"/>
+      <c r="V61" s="16"/>
+      <c r="W61" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="X61" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y61" s="16"/>
+      <c r="Z61" s="16"/>
+      <c r="AA61" s="16"/>
+      <c r="AB61" s="16"/>
+      <c r="AC61" s="16"/>
+      <c r="AD61" s="50"/>
+    </row>
+    <row r="62" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C62" s="51"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="16"/>
+      <c r="M62" s="16"/>
+      <c r="N62" s="16"/>
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
+      <c r="Q62" s="16"/>
+      <c r="R62" s="16"/>
+      <c r="S62" s="16"/>
+      <c r="T62" s="16"/>
+      <c r="U62" s="16"/>
+      <c r="V62" s="16"/>
+      <c r="W62" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="X62" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y62" s="16"/>
+      <c r="Z62" s="16"/>
+      <c r="AA62" s="16"/>
+      <c r="AB62" s="16"/>
+      <c r="AC62" s="16"/>
+      <c r="AD62" s="50"/>
+    </row>
+    <row r="63" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C63" s="52"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="53"/>
+      <c r="L63" s="53"/>
+      <c r="M63" s="53"/>
+      <c r="N63" s="53"/>
+      <c r="O63" s="53"/>
+      <c r="P63" s="53"/>
+      <c r="Q63" s="53"/>
+      <c r="R63" s="53"/>
+      <c r="S63" s="53"/>
+      <c r="T63" s="53"/>
+      <c r="U63" s="53"/>
+      <c r="V63" s="53"/>
+      <c r="W63" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="X63" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y63" s="53"/>
+      <c r="Z63" s="53"/>
+      <c r="AA63" s="53"/>
+      <c r="AB63" s="53"/>
+      <c r="AC63" s="53"/>
+      <c r="AD63" s="54"/>
+    </row>
+    <row r="64" spans="3:30" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C64" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" s="62"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="62"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="I64" s="62"/>
+      <c r="J64" s="62"/>
+      <c r="K64" s="62"/>
+      <c r="L64" s="62"/>
+      <c r="M64" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="N64" s="62"/>
+      <c r="O64" s="62"/>
+      <c r="P64" s="62"/>
+      <c r="Q64" s="62"/>
+      <c r="R64" s="62"/>
+      <c r="S64" s="62"/>
+      <c r="T64" s="62"/>
+      <c r="U64" s="62"/>
+      <c r="V64" s="62"/>
+      <c r="W64" s="62"/>
+      <c r="X64" s="62"/>
+      <c r="Y64" s="62"/>
+      <c r="Z64" s="62"/>
+      <c r="AA64" s="62"/>
+      <c r="AB64" s="62"/>
+      <c r="AC64" s="62"/>
+      <c r="AD64" s="64"/>
+    </row>
+    <row r="65" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C65" s="51"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
+      <c r="M65" s="16"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="16"/>
+      <c r="P65" s="16"/>
+      <c r="Q65" s="16"/>
+      <c r="R65" s="16"/>
+      <c r="S65" s="16"/>
+      <c r="T65" s="16"/>
+      <c r="U65" s="16"/>
+      <c r="V65" s="16"/>
+      <c r="W65" s="16"/>
+      <c r="X65" s="16"/>
+      <c r="Y65" s="16"/>
+      <c r="Z65" s="16"/>
+      <c r="AA65" s="16"/>
+      <c r="AB65" s="16"/>
+      <c r="AC65" s="16"/>
+      <c r="AD65" s="50"/>
+    </row>
+    <row r="66" spans="3:30" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C66" s="51"/>
+      <c r="D66" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" s="39">
+        <v>55</v>
+      </c>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="J66" s="39">
+        <v>55</v>
+      </c>
+      <c r="K66" s="16"/>
+      <c r="L66" s="16"/>
+      <c r="M66" s="16"/>
+      <c r="N66" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O66" s="39">
+        <v>55</v>
+      </c>
+      <c r="P66" s="16"/>
+      <c r="Q66" s="16"/>
+      <c r="R66" s="16"/>
+      <c r="S66" s="16"/>
+      <c r="T66" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="U66" s="16"/>
+      <c r="V66" s="16"/>
+      <c r="W66" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="X66" s="16"/>
+      <c r="Y66" s="16"/>
+      <c r="Z66" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA66" s="16"/>
+      <c r="AB66" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC66" s="16"/>
+      <c r="AD66" s="50"/>
+    </row>
+    <row r="67" spans="3:30" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C67" s="51"/>
+      <c r="D67" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="39">
+        <v>55</v>
+      </c>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J67" s="39">
+        <v>55</v>
+      </c>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="O67" s="39">
+        <v>55</v>
+      </c>
+      <c r="P67" s="16"/>
+      <c r="Q67" s="16"/>
+      <c r="R67" s="16"/>
+      <c r="S67" s="16"/>
+      <c r="T67" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="U67" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="V67" s="16"/>
+      <c r="W67" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="X67" s="16"/>
+      <c r="Y67" s="16"/>
+      <c r="Z67" s="16"/>
+      <c r="AA67" s="16"/>
+      <c r="AB67" s="16"/>
+      <c r="AC67" s="16"/>
+      <c r="AD67" s="50"/>
+    </row>
+    <row r="68" spans="3:30" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C68" s="51"/>
+      <c r="D68" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68" s="40">
+        <v>0.76470000000000005</v>
+      </c>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J68" s="40">
+        <v>0.72219999999999995</v>
+      </c>
+      <c r="K68" s="16"/>
+      <c r="L68" s="16"/>
+      <c r="M68" s="16"/>
+      <c r="N68" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="O68" s="40">
+        <v>0.76919999999999999</v>
+      </c>
+      <c r="P68" s="16"/>
+      <c r="Q68" s="16"/>
+      <c r="R68" s="16"/>
+      <c r="S68" s="16"/>
+      <c r="T68" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="U68" s="42">
+        <v>3</v>
+      </c>
+      <c r="V68" s="16"/>
+      <c r="W68" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="X68" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y68" s="16"/>
+      <c r="Z68" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA68" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB68" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC68" s="42">
+        <v>15</v>
+      </c>
+      <c r="AD68" s="50"/>
+    </row>
+    <row r="69" spans="3:30" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C69" s="51"/>
+      <c r="D69" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" s="40">
+        <v>0.86670000000000003</v>
+      </c>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="J69" s="40">
+        <v>0.76470000000000005</v>
+      </c>
+      <c r="K69" s="16"/>
+      <c r="L69" s="16"/>
+      <c r="M69" s="16"/>
+      <c r="N69" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="O69" s="40">
+        <v>0.625</v>
+      </c>
+      <c r="P69" s="16"/>
+      <c r="Q69" s="16"/>
+      <c r="R69" s="16"/>
+      <c r="S69" s="16"/>
+      <c r="T69" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="U69" s="42">
+        <v>2</v>
+      </c>
+      <c r="V69" s="16"/>
+      <c r="W69" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="X69" s="42">
+        <v>16</v>
+      </c>
+      <c r="Y69" s="16"/>
+      <c r="Z69" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA69" s="45" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="61" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="W61" s="43" t="s">
+      <c r="AB69" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC69" s="42">
+        <v>16</v>
+      </c>
+      <c r="AD69" s="50"/>
+    </row>
+    <row r="70" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C70" s="51"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="16"/>
+      <c r="M70" s="16"/>
+      <c r="N70" s="16"/>
+      <c r="O70" s="16"/>
+      <c r="P70" s="16"/>
+      <c r="Q70" s="16"/>
+      <c r="R70" s="16"/>
+      <c r="S70" s="16"/>
+      <c r="T70" s="16"/>
+      <c r="U70" s="16"/>
+      <c r="V70" s="16"/>
+      <c r="W70" s="16"/>
+      <c r="X70" s="16"/>
+      <c r="Y70" s="16"/>
+      <c r="Z70" s="16"/>
+      <c r="AA70" s="16"/>
+      <c r="AB70" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC70" s="42">
+        <v>0.3</v>
+      </c>
+      <c r="AD70" s="50"/>
+    </row>
+    <row r="71" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C71" s="51"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
+      <c r="M71" s="16"/>
+      <c r="N71" s="16"/>
+      <c r="O71" s="16"/>
+      <c r="P71" s="16"/>
+      <c r="Q71" s="16"/>
+      <c r="R71" s="16"/>
+      <c r="S71" s="16"/>
+      <c r="T71" s="16"/>
+      <c r="U71" s="16"/>
+      <c r="V71" s="16"/>
+      <c r="W71" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="X61" s="44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="W62" s="43" t="s">
+      <c r="X71" s="16"/>
+      <c r="Y71" s="16"/>
+      <c r="Z71" s="16"/>
+      <c r="AA71" s="16"/>
+      <c r="AB71" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC71" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD71" s="50"/>
+    </row>
+    <row r="72" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C72" s="51"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
+      <c r="J72" s="16"/>
+      <c r="K72" s="16"/>
+      <c r="L72" s="16"/>
+      <c r="M72" s="16"/>
+      <c r="N72" s="16"/>
+      <c r="O72" s="16"/>
+      <c r="P72" s="16"/>
+      <c r="Q72" s="16"/>
+      <c r="R72" s="16"/>
+      <c r="S72" s="16"/>
+      <c r="T72" s="16"/>
+      <c r="U72" s="16"/>
+      <c r="V72" s="16"/>
+      <c r="W72" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="X72" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y72" s="16"/>
+      <c r="Z72" s="16"/>
+      <c r="AA72" s="16"/>
+      <c r="AB72" s="16"/>
+      <c r="AC72" s="16"/>
+      <c r="AD72" s="50"/>
+    </row>
+    <row r="73" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C73" s="51"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16"/>
+      <c r="M73" s="16"/>
+      <c r="N73" s="16"/>
+      <c r="O73" s="16"/>
+      <c r="P73" s="16"/>
+      <c r="Q73" s="16"/>
+      <c r="R73" s="16"/>
+      <c r="S73" s="16"/>
+      <c r="T73" s="16"/>
+      <c r="U73" s="16"/>
+      <c r="V73" s="16"/>
+      <c r="W73" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="X73" s="42">
+        <v>16</v>
+      </c>
+      <c r="Y73" s="16"/>
+      <c r="Z73" s="16"/>
+      <c r="AA73" s="16"/>
+      <c r="AB73" s="16"/>
+      <c r="AC73" s="16"/>
+      <c r="AD73" s="50"/>
+    </row>
+    <row r="74" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C74" s="51"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="16"/>
+      <c r="M74" s="16"/>
+      <c r="N74" s="16"/>
+      <c r="O74" s="16"/>
+      <c r="P74" s="16"/>
+      <c r="Q74" s="16"/>
+      <c r="R74" s="16"/>
+      <c r="S74" s="16"/>
+      <c r="T74" s="16"/>
+      <c r="U74" s="16"/>
+      <c r="V74" s="16"/>
+      <c r="W74" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="X74" s="44">
+        <v>0.4</v>
+      </c>
+      <c r="Y74" s="16"/>
+      <c r="Z74" s="16"/>
+      <c r="AA74" s="16"/>
+      <c r="AB74" s="16"/>
+      <c r="AC74" s="16"/>
+      <c r="AD74" s="50"/>
+    </row>
+    <row r="75" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C75" s="51"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="16"/>
+      <c r="L75" s="16"/>
+      <c r="M75" s="16"/>
+      <c r="N75" s="16"/>
+      <c r="O75" s="16"/>
+      <c r="P75" s="16"/>
+      <c r="Q75" s="16"/>
+      <c r="R75" s="16"/>
+      <c r="S75" s="16"/>
+      <c r="T75" s="16"/>
+      <c r="U75" s="16"/>
+      <c r="V75" s="16"/>
+      <c r="W75" s="16"/>
+      <c r="X75" s="16"/>
+      <c r="Y75" s="16"/>
+      <c r="Z75" s="16"/>
+      <c r="AA75" s="16"/>
+      <c r="AB75" s="16"/>
+      <c r="AC75" s="16"/>
+      <c r="AD75" s="50"/>
+    </row>
+    <row r="76" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C76" s="51"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+      <c r="J76" s="16"/>
+      <c r="K76" s="16"/>
+      <c r="L76" s="16"/>
+      <c r="M76" s="16"/>
+      <c r="N76" s="16"/>
+      <c r="O76" s="16"/>
+      <c r="P76" s="16"/>
+      <c r="Q76" s="16"/>
+      <c r="R76" s="16"/>
+      <c r="S76" s="16"/>
+      <c r="T76" s="16"/>
+      <c r="U76" s="16"/>
+      <c r="V76" s="16"/>
+      <c r="W76" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="X76" s="16"/>
+      <c r="Y76" s="16"/>
+      <c r="Z76" s="16"/>
+      <c r="AA76" s="16"/>
+      <c r="AB76" s="16"/>
+      <c r="AC76" s="16"/>
+      <c r="AD76" s="50"/>
+    </row>
+    <row r="77" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C77" s="51"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="16"/>
+      <c r="K77" s="16"/>
+      <c r="L77" s="16"/>
+      <c r="M77" s="16"/>
+      <c r="N77" s="16"/>
+      <c r="O77" s="16"/>
+      <c r="P77" s="16"/>
+      <c r="Q77" s="16"/>
+      <c r="R77" s="16"/>
+      <c r="S77" s="16"/>
+      <c r="T77" s="16"/>
+      <c r="U77" s="16"/>
+      <c r="V77" s="16"/>
+      <c r="W77" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="X77" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y77" s="16"/>
+      <c r="Z77" s="16"/>
+      <c r="AA77" s="16"/>
+      <c r="AB77" s="16"/>
+      <c r="AC77" s="16"/>
+      <c r="AD77" s="50"/>
+    </row>
+    <row r="78" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C78" s="51"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="16"/>
+      <c r="J78" s="16"/>
+      <c r="K78" s="16"/>
+      <c r="L78" s="16"/>
+      <c r="M78" s="16"/>
+      <c r="N78" s="16"/>
+      <c r="O78" s="16"/>
+      <c r="P78" s="16"/>
+      <c r="Q78" s="16"/>
+      <c r="R78" s="16"/>
+      <c r="S78" s="16"/>
+      <c r="T78" s="16"/>
+      <c r="U78" s="16"/>
+      <c r="V78" s="16"/>
+      <c r="W78" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="X78" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y78" s="16"/>
+      <c r="Z78" s="16"/>
+      <c r="AA78" s="16"/>
+      <c r="AB78" s="16"/>
+      <c r="AC78" s="16"/>
+      <c r="AD78" s="50"/>
+    </row>
+    <row r="79" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C79" s="51"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+      <c r="J79" s="16"/>
+      <c r="K79" s="16"/>
+      <c r="L79" s="16"/>
+      <c r="M79" s="16"/>
+      <c r="N79" s="16"/>
+      <c r="O79" s="16"/>
+      <c r="P79" s="16"/>
+      <c r="Q79" s="16"/>
+      <c r="R79" s="16"/>
+      <c r="S79" s="16"/>
+      <c r="T79" s="16"/>
+      <c r="U79" s="16"/>
+      <c r="V79" s="16"/>
+      <c r="W79" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="X62" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="W63" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="X63" s="44" t="s">
-        <v>54</v>
-      </c>
+      <c r="X79" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y79" s="16"/>
+      <c r="Z79" s="16"/>
+      <c r="AA79" s="16"/>
+      <c r="AB79" s="16"/>
+      <c r="AC79" s="16"/>
+      <c r="AD79" s="50"/>
+    </row>
+    <row r="80" spans="3:30" x14ac:dyDescent="0.35">
+      <c r="C80" s="52"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="53"/>
+      <c r="F80" s="53"/>
+      <c r="G80" s="53"/>
+      <c r="H80" s="53"/>
+      <c r="I80" s="53"/>
+      <c r="J80" s="53"/>
+      <c r="K80" s="53"/>
+      <c r="L80" s="53"/>
+      <c r="M80" s="53"/>
+      <c r="N80" s="53"/>
+      <c r="O80" s="53"/>
+      <c r="P80" s="53"/>
+      <c r="Q80" s="53"/>
+      <c r="R80" s="53"/>
+      <c r="S80" s="53"/>
+      <c r="T80" s="53"/>
+      <c r="U80" s="53"/>
+      <c r="V80" s="53"/>
+      <c r="W80" s="53"/>
+      <c r="X80" s="53"/>
+      <c r="Y80" s="53"/>
+      <c r="Z80" s="53"/>
+      <c r="AA80" s="53"/>
+      <c r="AB80" s="53"/>
+      <c r="AC80" s="53"/>
+      <c r="AD80" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created sep critical csvs
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312225C7-B67E-4FEB-8BC9-31B35D96E3BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAAB233-B9A2-4DE5-8B21-D8DCE11F6552}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -1117,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
   <dimension ref="B2:AD80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="52" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updates to critical EDA
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAAB233-B9A2-4DE5-8B21-D8DCE11F6552}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89647868-78FB-42CF-968A-781DDC225EEA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -1117,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
   <dimension ref="B2:AD80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:F40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1546,6 +1546,14 @@
       </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <f>SUM(F7:F10)</f>
+        <v>390</v>
+      </c>
+      <c r="H11">
+        <f>SUM(H7:H10)</f>
+        <v>33975</v>
+      </c>
       <c r="K11" s="18"/>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>

</xml_diff>

<commit_message>
adding csv with word2vec embeddings
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E1B2AC-872B-4890-9173-05EE570726C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68B8610-9F0B-47C7-911B-286F60D64164}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -926,13 +926,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1249,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
   <dimension ref="B2:AD80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L5" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1698,13 +1698,13 @@
       <c r="N11" s="79">
         <v>24</v>
       </c>
-      <c r="O11" s="80">
+      <c r="O11" s="82">
         <v>2</v>
       </c>
       <c r="P11" s="79">
         <v>0</v>
       </c>
-      <c r="Q11" s="81">
+      <c r="Q11" s="80">
         <f>SUM(L11:P11)</f>
         <v>161</v>
       </c>
@@ -1729,7 +1729,7 @@
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
       <c r="P12" s="15"/>
-      <c r="Q12" s="82">
+      <c r="Q12" s="81">
         <f>SUM(Q6:Q11)</f>
         <v>1333</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="R31" s="15"/>
       <c r="S31" s="47"/>
     </row>
-    <row r="32" spans="2:26" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B32" s="48"/>
       <c r="C32" s="15"/>
       <c r="D32" s="34"/>

</xml_diff>

<commit_message>
SVM, LSTM and Covnet for Word2Vec complete and working
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68B8610-9F0B-47C7-911B-286F60D64164}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0975A4-2803-4CB2-B3F9-C85DE8539318}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="102">
   <si>
     <t>Low</t>
   </si>
@@ -259,13 +259,91 @@
   </si>
   <si>
     <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>1. RNN LSTM Word2Vec Quake (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>2. RNN LSTM Word2Vec Quake (Medium Vs Critical)</t>
+  </si>
+  <si>
+    <t>1. SVM SGD Word2Vec Quake (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. SVM SGD Word2Vec Quake (Med Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. SVM SGD Word2Vec Quake (High Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. SVM SGD Word2Vec FLood (Med Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. SVM SGD Word2Vec FLood (High Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. RNN LSTM Word2Vec Quake (High Vs Critical)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>1D Cov</t>
+  </si>
+  <si>
+    <t>Neurons/Filters</t>
+  </si>
+  <si>
+    <t>Patch-size</t>
+  </si>
+  <si>
+    <t>Relu</t>
+  </si>
+  <si>
+    <t>1. RNN LSTM Word2Vec FLood (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>1. 1D CNN Embeddings  Flood (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. RNN LSTM Word2Vec Flood (Medium Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. 1D CNN Embeddings Flood (Med Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. RNN LSTM Word2Vec Flood (High Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. 1D CNN Embeddings Flood (High Vs Critical)</t>
+  </si>
+  <si>
+    <t>1. 1D CNN Embeddings Quake (Low Vs Critical)</t>
+  </si>
+  <si>
+    <t>2. 1D CNN Embeddings Quake (Med Vs Critical)</t>
+  </si>
+  <si>
+    <t>3. 1D CNN Embeddings Quake (High Vs Critical)</t>
+  </si>
+  <si>
+    <t>RMSprop - lr = 0.001</t>
+  </si>
+  <si>
+    <t>lr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,6 +437,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -410,7 +503,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -759,11 +852,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -932,6 +1131,28 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1247,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
-  <dimension ref="B2:AD80"/>
+  <dimension ref="B2:AP171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="42" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J152" sqref="J152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1259,8 +1480,10 @@
     <col min="4" max="4" width="19.453125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="17.08984375" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" customWidth="1"/>
     <col min="11" max="11" width="15.08984375" customWidth="1"/>
     <col min="14" max="14" width="17.81640625" customWidth="1"/>
+    <col min="16" max="16" width="20.81640625" customWidth="1"/>
     <col min="20" max="20" width="29.6328125" customWidth="1"/>
     <col min="21" max="21" width="29.1796875" customWidth="1"/>
     <col min="23" max="23" width="21.08984375" customWidth="1"/>
@@ -1268,6 +1491,11 @@
     <col min="26" max="26" width="14.26953125" customWidth="1"/>
     <col min="27" max="27" width="21" customWidth="1"/>
     <col min="28" max="28" width="11.81640625" customWidth="1"/>
+    <col min="29" max="29" width="16.7265625" customWidth="1"/>
+    <col min="33" max="33" width="20.6328125" customWidth="1"/>
+    <col min="34" max="34" width="20.81640625" customWidth="1"/>
+    <col min="37" max="37" width="33.7265625" customWidth="1"/>
+    <col min="42" max="42" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="26" x14ac:dyDescent="0.6">
@@ -3854,6 +4082,3519 @@
       <c r="AC80" s="50"/>
       <c r="AD80" s="51"/>
     </row>
+    <row r="83" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="84" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C84" s="87"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16"/>
+      <c r="K84" s="16"/>
+      <c r="L84" s="16"/>
+      <c r="M84" s="16"/>
+      <c r="N84" s="16"/>
+      <c r="O84" s="16"/>
+      <c r="P84" s="16"/>
+      <c r="Q84" s="16"/>
+      <c r="R84" s="16"/>
+      <c r="S84" s="16"/>
+      <c r="T84" s="16"/>
+      <c r="U84" s="16"/>
+      <c r="V84" s="16"/>
+      <c r="W84" s="16"/>
+      <c r="X84" s="16"/>
+      <c r="Y84" s="16"/>
+      <c r="Z84" s="16"/>
+      <c r="AA84" s="16"/>
+      <c r="AB84" s="16"/>
+      <c r="AC84" s="22"/>
+      <c r="AG84" s="87"/>
+      <c r="AH84" s="16"/>
+      <c r="AI84" s="16"/>
+      <c r="AJ84" s="16"/>
+      <c r="AK84" s="16"/>
+      <c r="AL84" s="16"/>
+      <c r="AM84" s="16"/>
+      <c r="AN84" s="16"/>
+      <c r="AO84" s="16"/>
+      <c r="AP84" s="22"/>
+    </row>
+    <row r="85" spans="3:42" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C85" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15"/>
+      <c r="S85" s="15"/>
+      <c r="T85" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="U85" s="15"/>
+      <c r="V85" s="15"/>
+      <c r="W85" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="X85" s="15"/>
+      <c r="Y85" s="15"/>
+      <c r="Z85" s="15"/>
+      <c r="AA85" s="15"/>
+      <c r="AB85" s="15"/>
+      <c r="AC85" s="17"/>
+      <c r="AG85" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH85" s="15"/>
+      <c r="AI85" s="15"/>
+      <c r="AJ85" s="15"/>
+      <c r="AK85" s="15"/>
+      <c r="AL85" s="15"/>
+      <c r="AM85" s="15"/>
+      <c r="AN85" s="15"/>
+      <c r="AO85" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP85" s="17"/>
+    </row>
+    <row r="86" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C86" s="89"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="48"/>
+      <c r="N86" s="15"/>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="R86" s="15"/>
+      <c r="S86" s="15"/>
+      <c r="T86" s="15"/>
+      <c r="U86" s="15"/>
+      <c r="V86" s="15"/>
+      <c r="W86" s="48"/>
+      <c r="X86" s="15"/>
+      <c r="Y86" s="15"/>
+      <c r="Z86" s="15"/>
+      <c r="AA86" s="15"/>
+      <c r="AB86" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC86" s="17"/>
+      <c r="AG86" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH86" s="15"/>
+      <c r="AI86" s="15"/>
+      <c r="AJ86" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK86" s="15"/>
+      <c r="AL86" s="15"/>
+      <c r="AM86" s="15"/>
+      <c r="AN86" s="15"/>
+      <c r="AO86" s="15"/>
+      <c r="AP86" s="17"/>
+    </row>
+    <row r="87" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C87" s="89"/>
+      <c r="D87" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E87" s="36">
+        <v>25</v>
+      </c>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="J87" s="39">
+        <v>200</v>
+      </c>
+      <c r="K87" s="15"/>
+      <c r="L87" s="15"/>
+      <c r="M87" s="48"/>
+      <c r="N87" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="O87" s="36">
+        <v>25</v>
+      </c>
+      <c r="P87" s="15"/>
+      <c r="Q87" s="15"/>
+      <c r="R87" s="15"/>
+      <c r="S87" s="15"/>
+      <c r="T87" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="U87" s="39">
+        <v>200</v>
+      </c>
+      <c r="V87" s="15"/>
+      <c r="W87" s="48"/>
+      <c r="X87" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y87" s="36">
+        <v>25</v>
+      </c>
+      <c r="Z87" s="15"/>
+      <c r="AA87" s="15"/>
+      <c r="AB87" s="15"/>
+      <c r="AC87" s="17"/>
+      <c r="AG87" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH87" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI87" s="15"/>
+      <c r="AJ87" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK87" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL87" s="15"/>
+      <c r="AM87" s="15"/>
+      <c r="AN87" s="15"/>
+      <c r="AO87" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP87" s="90" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C88" s="89"/>
+      <c r="D88" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="36">
+        <v>25</v>
+      </c>
+      <c r="F88" s="15"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="J88" s="39">
+        <v>2</v>
+      </c>
+      <c r="K88" s="15"/>
+      <c r="L88" s="15"/>
+      <c r="M88" s="48"/>
+      <c r="N88" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="O88" s="36">
+        <v>25</v>
+      </c>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+      <c r="R88" s="15"/>
+      <c r="S88" s="15"/>
+      <c r="T88" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="U88" s="39">
+        <v>2</v>
+      </c>
+      <c r="V88" s="15"/>
+      <c r="W88" s="48"/>
+      <c r="X88" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y88" s="36">
+        <v>25</v>
+      </c>
+      <c r="Z88" s="15"/>
+      <c r="AA88" s="15"/>
+      <c r="AB88" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC88" s="90">
+        <v>200</v>
+      </c>
+      <c r="AG88" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH88" s="39">
+        <v>8</v>
+      </c>
+      <c r="AI88" s="15"/>
+      <c r="AJ88" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK88" s="39">
+        <v>4</v>
+      </c>
+      <c r="AL88" s="15"/>
+      <c r="AM88" s="15"/>
+      <c r="AN88" s="15"/>
+      <c r="AO88" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP88" s="90" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C89" s="89"/>
+      <c r="D89" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E89" s="37">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="F89" s="15"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="J89" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="K89" s="15"/>
+      <c r="L89" s="15"/>
+      <c r="M89" s="48"/>
+      <c r="N89" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="O89" s="37">
+        <v>0.85709999999999997</v>
+      </c>
+      <c r="P89" s="15"/>
+      <c r="Q89" s="15"/>
+      <c r="R89" s="15"/>
+      <c r="S89" s="15"/>
+      <c r="T89" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="U89" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="V89" s="15"/>
+      <c r="W89" s="48"/>
+      <c r="X89" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y89" s="37">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="Z89" s="15"/>
+      <c r="AA89" s="15"/>
+      <c r="AB89" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC89" s="90">
+        <v>2</v>
+      </c>
+      <c r="AG89" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH89" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI89" s="15"/>
+      <c r="AJ89" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK89" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL89" s="15"/>
+      <c r="AM89" s="15"/>
+      <c r="AN89" s="15"/>
+      <c r="AO89" s="15"/>
+      <c r="AP89" s="17"/>
+    </row>
+    <row r="90" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C90" s="89"/>
+      <c r="D90" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E90" s="37">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="F90" s="15"/>
+      <c r="G90" s="15"/>
+      <c r="H90" s="15"/>
+      <c r="I90" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="J90" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K90" s="15"/>
+      <c r="L90" s="15"/>
+      <c r="M90" s="48"/>
+      <c r="N90" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O90" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="P90" s="15"/>
+      <c r="Q90" s="15"/>
+      <c r="R90" s="15"/>
+      <c r="S90" s="15"/>
+      <c r="T90" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="U90" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="V90" s="15"/>
+      <c r="W90" s="48"/>
+      <c r="X90" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y90" s="37">
+        <v>0.45450000000000002</v>
+      </c>
+      <c r="Z90" s="15"/>
+      <c r="AA90" s="15"/>
+      <c r="AB90" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC90" s="90">
+        <v>0.3</v>
+      </c>
+      <c r="AG90" s="89"/>
+      <c r="AH90" s="15"/>
+      <c r="AI90" s="15"/>
+      <c r="AJ90" s="15"/>
+      <c r="AK90" s="15"/>
+      <c r="AL90" s="15"/>
+      <c r="AM90" s="15"/>
+      <c r="AN90" s="15"/>
+      <c r="AO90" s="15"/>
+      <c r="AP90" s="17"/>
+    </row>
+    <row r="91" spans="3:42" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C91" s="89"/>
+      <c r="D91" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="E91" s="84">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="F91" s="15"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="15"/>
+      <c r="M91" s="48"/>
+      <c r="N91" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="O91" s="84">
+        <v>0.5333</v>
+      </c>
+      <c r="P91" s="15"/>
+      <c r="Q91" s="15"/>
+      <c r="R91" s="15"/>
+      <c r="S91" s="15"/>
+      <c r="T91" s="15"/>
+      <c r="U91" s="15"/>
+      <c r="V91" s="15"/>
+      <c r="W91" s="48"/>
+      <c r="X91" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y91" s="84">
+        <v>0.4667</v>
+      </c>
+      <c r="Z91" s="15"/>
+      <c r="AA91" s="15"/>
+      <c r="AB91" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC91" s="90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD91" s="15"/>
+      <c r="AE91" s="15"/>
+      <c r="AG91" s="95" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH91" s="15"/>
+      <c r="AI91" s="15"/>
+      <c r="AJ91" s="15"/>
+      <c r="AK91" s="15"/>
+      <c r="AL91" s="15"/>
+      <c r="AM91" s="15"/>
+      <c r="AN91" s="15"/>
+      <c r="AO91" s="15"/>
+      <c r="AP91" s="17"/>
+    </row>
+    <row r="92" spans="3:42" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C92" s="89"/>
+      <c r="D92" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="E92" s="84">
+        <v>0.91069999999999995</v>
+      </c>
+      <c r="F92" s="15"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="48"/>
+      <c r="N92" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="O92" s="84">
+        <v>0.58040000000000003</v>
+      </c>
+      <c r="P92" s="15"/>
+      <c r="Q92" s="15"/>
+      <c r="R92" s="15"/>
+      <c r="S92" s="15"/>
+      <c r="T92" s="15"/>
+      <c r="U92" s="15"/>
+      <c r="V92" s="15"/>
+      <c r="W92" s="48"/>
+      <c r="X92" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y92" s="84">
+        <v>0.54459999999999997</v>
+      </c>
+      <c r="Z92" s="15"/>
+      <c r="AA92" s="15"/>
+      <c r="AB92" s="15"/>
+      <c r="AC92" s="17"/>
+      <c r="AG92" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH92" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI92" s="15"/>
+      <c r="AJ92" s="15"/>
+      <c r="AK92" s="15"/>
+      <c r="AL92" s="15"/>
+      <c r="AM92" s="15"/>
+      <c r="AN92" s="15"/>
+      <c r="AO92" s="15"/>
+      <c r="AP92" s="17"/>
+    </row>
+    <row r="93" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C93" s="89"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="15"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="15"/>
+      <c r="M93" s="15"/>
+      <c r="N93" s="15"/>
+      <c r="O93" s="15"/>
+      <c r="P93" s="15"/>
+      <c r="Q93" s="15"/>
+      <c r="R93" s="15"/>
+      <c r="S93" s="15"/>
+      <c r="T93" s="15"/>
+      <c r="U93" s="15"/>
+      <c r="V93" s="15"/>
+      <c r="W93" s="15"/>
+      <c r="X93" s="15"/>
+      <c r="Y93" s="15"/>
+      <c r="Z93" s="15"/>
+      <c r="AA93" s="15"/>
+      <c r="AB93" s="15"/>
+      <c r="AC93" s="17"/>
+      <c r="AG93" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH93" s="39">
+        <v>1</v>
+      </c>
+      <c r="AI93" s="15"/>
+      <c r="AJ93" s="15"/>
+      <c r="AK93" s="15"/>
+      <c r="AL93" s="15"/>
+      <c r="AM93" s="15"/>
+      <c r="AN93" s="15"/>
+      <c r="AO93" s="15"/>
+      <c r="AP93" s="17"/>
+    </row>
+    <row r="94" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C94" s="91"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="50"/>
+      <c r="F94" s="50"/>
+      <c r="G94" s="50"/>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
+      <c r="L94" s="15"/>
+      <c r="M94" s="15"/>
+      <c r="N94" s="15"/>
+      <c r="O94" s="15"/>
+      <c r="P94" s="15"/>
+      <c r="Q94" s="15"/>
+      <c r="R94" s="15"/>
+      <c r="S94" s="15"/>
+      <c r="T94" s="15"/>
+      <c r="U94" s="15"/>
+      <c r="V94" s="15"/>
+      <c r="W94" s="15"/>
+      <c r="X94" s="15"/>
+      <c r="Y94" s="15"/>
+      <c r="Z94" s="15"/>
+      <c r="AA94" s="15"/>
+      <c r="AB94" s="15"/>
+      <c r="AC94" s="17"/>
+      <c r="AG94" s="97" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH94" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI94" s="50"/>
+      <c r="AJ94" s="50"/>
+      <c r="AK94" s="50"/>
+      <c r="AL94" s="15"/>
+      <c r="AM94" s="15"/>
+      <c r="AN94" s="15"/>
+      <c r="AO94" s="15"/>
+      <c r="AP94" s="17"/>
+    </row>
+    <row r="95" spans="3:42" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C95" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="D95" s="59"/>
+      <c r="E95" s="59"/>
+      <c r="F95" s="59"/>
+      <c r="G95" s="59"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="15"/>
+      <c r="M95" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="N95" s="59"/>
+      <c r="O95" s="59"/>
+      <c r="P95" s="59"/>
+      <c r="Q95" s="59"/>
+      <c r="R95" s="15"/>
+      <c r="S95" s="15"/>
+      <c r="T95" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="U95" s="15"/>
+      <c r="V95" s="15"/>
+      <c r="W95" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="X95" s="59"/>
+      <c r="Y95" s="59"/>
+      <c r="Z95" s="59"/>
+      <c r="AA95" s="59"/>
+      <c r="AB95" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC95" s="17"/>
+      <c r="AG95" s="89"/>
+      <c r="AH95" s="15"/>
+      <c r="AI95" s="15"/>
+      <c r="AJ95" s="15"/>
+      <c r="AK95" s="15"/>
+      <c r="AL95" s="15"/>
+      <c r="AM95" s="15"/>
+      <c r="AN95" s="15"/>
+      <c r="AO95" s="15"/>
+      <c r="AP95" s="17"/>
+    </row>
+    <row r="96" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C96" s="89"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="15"/>
+      <c r="L96" s="15"/>
+      <c r="M96" s="48"/>
+      <c r="N96" s="15"/>
+      <c r="O96" s="15"/>
+      <c r="P96" s="15"/>
+      <c r="Q96" s="15"/>
+      <c r="R96" s="15"/>
+      <c r="S96" s="15"/>
+      <c r="T96" s="15"/>
+      <c r="U96" s="15"/>
+      <c r="V96" s="15"/>
+      <c r="W96" s="48"/>
+      <c r="X96" s="15"/>
+      <c r="Y96" s="15"/>
+      <c r="Z96" s="15"/>
+      <c r="AA96" s="15"/>
+      <c r="AB96" s="15"/>
+      <c r="AC96" s="17"/>
+      <c r="AG96" s="89"/>
+      <c r="AH96" s="15"/>
+      <c r="AI96" s="15"/>
+      <c r="AJ96" s="15"/>
+      <c r="AK96" s="15"/>
+      <c r="AL96" s="15"/>
+      <c r="AM96" s="15"/>
+      <c r="AN96" s="15"/>
+      <c r="AO96" s="15"/>
+      <c r="AP96" s="17"/>
+    </row>
+    <row r="97" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C97" s="89"/>
+      <c r="D97" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E97" s="36">
+        <v>25</v>
+      </c>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="J97" s="39">
+        <v>100</v>
+      </c>
+      <c r="K97" s="15"/>
+      <c r="L97" s="15"/>
+      <c r="M97" s="48"/>
+      <c r="N97" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="O97" s="36">
+        <v>25</v>
+      </c>
+      <c r="P97" s="15"/>
+      <c r="Q97" s="15"/>
+      <c r="R97" s="15"/>
+      <c r="S97" s="15"/>
+      <c r="T97" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="U97" s="39">
+        <v>100</v>
+      </c>
+      <c r="V97" s="15"/>
+      <c r="W97" s="48"/>
+      <c r="X97" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y97" s="36">
+        <v>25</v>
+      </c>
+      <c r="Z97" s="15"/>
+      <c r="AA97" s="15"/>
+      <c r="AB97" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC97" s="90">
+        <v>100</v>
+      </c>
+      <c r="AG97" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH97" s="15"/>
+      <c r="AI97" s="15"/>
+      <c r="AJ97" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK97" s="15"/>
+      <c r="AL97" s="15"/>
+      <c r="AM97" s="15"/>
+      <c r="AN97" s="15"/>
+      <c r="AO97" s="15"/>
+      <c r="AP97" s="17"/>
+    </row>
+    <row r="98" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C98" s="89"/>
+      <c r="D98" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="36">
+        <v>25</v>
+      </c>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="J98" s="39">
+        <v>2</v>
+      </c>
+      <c r="K98" s="15"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="48"/>
+      <c r="N98" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="O98" s="36">
+        <v>25</v>
+      </c>
+      <c r="P98" s="15"/>
+      <c r="Q98" s="15"/>
+      <c r="R98" s="15"/>
+      <c r="S98" s="15"/>
+      <c r="T98" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="U98" s="39">
+        <v>2</v>
+      </c>
+      <c r="V98" s="15"/>
+      <c r="W98" s="48"/>
+      <c r="X98" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y98" s="36">
+        <v>25</v>
+      </c>
+      <c r="Z98" s="15"/>
+      <c r="AA98" s="15"/>
+      <c r="AB98" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC98" s="90">
+        <v>2</v>
+      </c>
+      <c r="AG98" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH98" s="15"/>
+      <c r="AI98" s="15"/>
+      <c r="AJ98" s="15"/>
+      <c r="AK98" s="15"/>
+      <c r="AL98" s="15"/>
+      <c r="AM98" s="15"/>
+      <c r="AN98" s="15"/>
+      <c r="AO98" s="15"/>
+      <c r="AP98" s="17"/>
+    </row>
+    <row r="99" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C99" s="89"/>
+      <c r="D99" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E99" s="37">
+        <v>0.85709999999999997</v>
+      </c>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="J99" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="K99" s="15"/>
+      <c r="L99" s="15"/>
+      <c r="M99" s="48"/>
+      <c r="N99" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="O99" s="37">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="P99" s="15"/>
+      <c r="Q99" s="15"/>
+      <c r="R99" s="15"/>
+      <c r="S99" s="15"/>
+      <c r="T99" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="U99" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="V99" s="15"/>
+      <c r="W99" s="48"/>
+      <c r="X99" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y99" s="37">
+        <v>0.57140000000000002</v>
+      </c>
+      <c r="Z99" s="15"/>
+      <c r="AA99" s="15"/>
+      <c r="AB99" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC99" s="90">
+        <v>0.3</v>
+      </c>
+      <c r="AG99" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH99" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI99" s="15"/>
+      <c r="AJ99" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK99" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL99" s="15"/>
+      <c r="AM99" s="15"/>
+      <c r="AN99" s="15"/>
+      <c r="AO99" s="15"/>
+      <c r="AP99" s="17"/>
+    </row>
+    <row r="100" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C100" s="89"/>
+      <c r="D100" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E100" s="37">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
+      <c r="I100" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="J100" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K100" s="15"/>
+      <c r="L100" s="15"/>
+      <c r="M100" s="48"/>
+      <c r="N100" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O100" s="37">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="P100" s="15"/>
+      <c r="Q100" s="15"/>
+      <c r="R100" s="15"/>
+      <c r="S100" s="15"/>
+      <c r="T100" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="U100" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="V100" s="15"/>
+      <c r="W100" s="48"/>
+      <c r="X100" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y100" s="37">
+        <v>0.57140000000000002</v>
+      </c>
+      <c r="Z100" s="15"/>
+      <c r="AA100" s="15"/>
+      <c r="AB100" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC100" s="90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG100" s="96" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH100" s="39">
+        <v>16</v>
+      </c>
+      <c r="AI100" s="15"/>
+      <c r="AJ100" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK100" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL100" s="15"/>
+      <c r="AM100" s="15"/>
+      <c r="AN100" s="15"/>
+      <c r="AO100" s="15"/>
+      <c r="AP100" s="17"/>
+    </row>
+    <row r="101" spans="3:42" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C101" s="89"/>
+      <c r="D101" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="E101" s="84">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="F101" s="15"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15"/>
+      <c r="J101" s="15"/>
+      <c r="K101" s="15"/>
+      <c r="L101" s="15"/>
+      <c r="M101" s="48"/>
+      <c r="N101" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="O101" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="P101" s="15"/>
+      <c r="Q101" s="15"/>
+      <c r="R101" s="15"/>
+      <c r="S101" s="15"/>
+      <c r="T101" s="15"/>
+      <c r="U101" s="15"/>
+      <c r="V101" s="15"/>
+      <c r="W101" s="48"/>
+      <c r="X101" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y101" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="Z101" s="15"/>
+      <c r="AA101" s="15"/>
+      <c r="AB101" s="15"/>
+      <c r="AC101" s="17"/>
+      <c r="AG101" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH101" s="39">
+        <v>3</v>
+      </c>
+      <c r="AI101" s="15"/>
+      <c r="AJ101" s="15"/>
+      <c r="AK101" s="15"/>
+      <c r="AL101" s="15"/>
+      <c r="AM101" s="15"/>
+      <c r="AN101" s="15"/>
+      <c r="AO101" s="15"/>
+      <c r="AP101" s="17"/>
+    </row>
+    <row r="102" spans="3:42" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C102" s="89"/>
+      <c r="D102" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="E102" s="84">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="15"/>
+      <c r="I102" s="15"/>
+      <c r="J102" s="15"/>
+      <c r="K102" s="15"/>
+      <c r="L102" s="15"/>
+      <c r="M102" s="48"/>
+      <c r="N102" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="O102" s="84">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="P102" s="15"/>
+      <c r="Q102" s="15"/>
+      <c r="R102" s="15"/>
+      <c r="S102" s="15"/>
+      <c r="T102" s="15"/>
+      <c r="U102" s="15"/>
+      <c r="V102" s="15"/>
+      <c r="W102" s="48"/>
+      <c r="X102" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y102" s="84">
+        <v>0.625</v>
+      </c>
+      <c r="Z102" s="15"/>
+      <c r="AA102" s="15"/>
+      <c r="AB102" s="15"/>
+      <c r="AC102" s="17"/>
+      <c r="AG102" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH102" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI102" s="15"/>
+      <c r="AJ102" s="15"/>
+      <c r="AK102" s="15"/>
+      <c r="AL102" s="15"/>
+      <c r="AM102" s="15"/>
+      <c r="AN102" s="15"/>
+      <c r="AO102" s="15"/>
+      <c r="AP102" s="17"/>
+    </row>
+    <row r="103" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C103" s="89"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="15"/>
+      <c r="I103" s="15"/>
+      <c r="J103" s="15"/>
+      <c r="K103" s="15"/>
+      <c r="L103" s="15"/>
+      <c r="M103" s="48"/>
+      <c r="N103" s="15"/>
+      <c r="O103" s="15"/>
+      <c r="P103" s="15"/>
+      <c r="Q103" s="15"/>
+      <c r="R103" s="15"/>
+      <c r="S103" s="15"/>
+      <c r="T103" s="15"/>
+      <c r="U103" s="15"/>
+      <c r="V103" s="15"/>
+      <c r="W103" s="48"/>
+      <c r="X103" s="15"/>
+      <c r="Y103" s="15"/>
+      <c r="Z103" s="15"/>
+      <c r="AA103" s="15"/>
+      <c r="AB103" s="15"/>
+      <c r="AC103" s="17"/>
+      <c r="AG103" s="89"/>
+      <c r="AH103" s="15"/>
+      <c r="AI103" s="15"/>
+      <c r="AJ103" s="15"/>
+      <c r="AK103" s="15"/>
+      <c r="AL103" s="15"/>
+      <c r="AM103" s="15"/>
+      <c r="AN103" s="15"/>
+      <c r="AO103" s="15"/>
+      <c r="AP103" s="17"/>
+    </row>
+    <row r="104" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C104" s="89"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="15"/>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="15"/>
+      <c r="L104" s="15"/>
+      <c r="M104" s="15"/>
+      <c r="N104" s="15"/>
+      <c r="O104" s="15"/>
+      <c r="P104" s="15"/>
+      <c r="Q104" s="15"/>
+      <c r="R104" s="15"/>
+      <c r="S104" s="15"/>
+      <c r="T104" s="15"/>
+      <c r="U104" s="15"/>
+      <c r="V104" s="15"/>
+      <c r="W104" s="15"/>
+      <c r="X104" s="15"/>
+      <c r="Y104" s="15"/>
+      <c r="Z104" s="15"/>
+      <c r="AA104" s="15"/>
+      <c r="AB104" s="15"/>
+      <c r="AC104" s="17"/>
+      <c r="AG104" s="95" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH104" s="15"/>
+      <c r="AI104" s="15"/>
+      <c r="AJ104" s="15"/>
+      <c r="AK104" s="15"/>
+      <c r="AL104" s="15"/>
+      <c r="AM104" s="15"/>
+      <c r="AN104" s="15"/>
+      <c r="AO104" s="15"/>
+      <c r="AP104" s="17"/>
+    </row>
+    <row r="105" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C105" s="89"/>
+      <c r="D105" s="15"/>
+      <c r="E105" s="15"/>
+      <c r="F105" s="15"/>
+      <c r="G105" s="15"/>
+      <c r="H105" s="15"/>
+      <c r="I105" s="15"/>
+      <c r="J105" s="15"/>
+      <c r="K105" s="15"/>
+      <c r="L105" s="15"/>
+      <c r="M105" s="15"/>
+      <c r="N105" s="15"/>
+      <c r="O105" s="15"/>
+      <c r="P105" s="15"/>
+      <c r="Q105" s="15"/>
+      <c r="R105" s="15"/>
+      <c r="S105" s="15"/>
+      <c r="T105" s="15"/>
+      <c r="U105" s="15"/>
+      <c r="V105" s="15"/>
+      <c r="W105" s="15"/>
+      <c r="X105" s="15"/>
+      <c r="Y105" s="15"/>
+      <c r="Z105" s="15"/>
+      <c r="AA105" s="15"/>
+      <c r="AB105" s="15"/>
+      <c r="AC105" s="17"/>
+      <c r="AG105" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH105" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI105" s="15"/>
+      <c r="AJ105" s="15"/>
+      <c r="AK105" s="15"/>
+      <c r="AL105" s="15"/>
+      <c r="AM105" s="15"/>
+      <c r="AN105" s="15"/>
+      <c r="AO105" s="15"/>
+      <c r="AP105" s="17"/>
+    </row>
+    <row r="106" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C106" s="89"/>
+      <c r="D106" s="15"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="15"/>
+      <c r="H106" s="15"/>
+      <c r="I106" s="15"/>
+      <c r="J106" s="15"/>
+      <c r="K106" s="15"/>
+      <c r="L106" s="15"/>
+      <c r="M106" s="15"/>
+      <c r="N106" s="15"/>
+      <c r="O106" s="15"/>
+      <c r="P106" s="15"/>
+      <c r="Q106" s="15"/>
+      <c r="R106" s="15"/>
+      <c r="S106" s="15"/>
+      <c r="T106" s="15"/>
+      <c r="U106" s="15"/>
+      <c r="V106" s="15"/>
+      <c r="W106" s="15"/>
+      <c r="X106" s="15"/>
+      <c r="Y106" s="15"/>
+      <c r="Z106" s="15"/>
+      <c r="AA106" s="15"/>
+      <c r="AB106" s="15"/>
+      <c r="AC106" s="17"/>
+      <c r="AG106" s="96" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH106" s="39">
+        <v>8</v>
+      </c>
+      <c r="AI106" s="15"/>
+      <c r="AJ106" s="15"/>
+      <c r="AK106" s="15"/>
+      <c r="AL106" s="15"/>
+      <c r="AM106" s="15"/>
+      <c r="AN106" s="15"/>
+      <c r="AO106" s="15"/>
+      <c r="AP106" s="17"/>
+    </row>
+    <row r="107" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C107" s="18"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="19"/>
+      <c r="J107" s="19"/>
+      <c r="K107" s="19"/>
+      <c r="L107" s="19"/>
+      <c r="M107" s="19"/>
+      <c r="N107" s="19"/>
+      <c r="O107" s="19"/>
+      <c r="P107" s="19"/>
+      <c r="Q107" s="19"/>
+      <c r="R107" s="19"/>
+      <c r="S107" s="19"/>
+      <c r="T107" s="19"/>
+      <c r="U107" s="19"/>
+      <c r="V107" s="19"/>
+      <c r="W107" s="19"/>
+      <c r="X107" s="19"/>
+      <c r="Y107" s="19"/>
+      <c r="Z107" s="19"/>
+      <c r="AA107" s="19"/>
+      <c r="AB107" s="19"/>
+      <c r="AC107" s="21"/>
+      <c r="AG107" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH107" s="39">
+        <v>3</v>
+      </c>
+      <c r="AI107" s="15"/>
+      <c r="AJ107" s="15"/>
+      <c r="AK107" s="15"/>
+      <c r="AL107" s="15"/>
+      <c r="AM107" s="15"/>
+      <c r="AN107" s="15"/>
+      <c r="AO107" s="15"/>
+      <c r="AP107" s="17"/>
+    </row>
+    <row r="108" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="AG108" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH108" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI108" s="15"/>
+      <c r="AJ108" s="15"/>
+      <c r="AK108" s="15"/>
+      <c r="AL108" s="15"/>
+      <c r="AM108" s="15"/>
+      <c r="AN108" s="15"/>
+      <c r="AO108" s="15"/>
+      <c r="AP108" s="17"/>
+    </row>
+    <row r="109" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="AG109" s="95" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH109" s="15"/>
+      <c r="AI109" s="15"/>
+      <c r="AJ109" s="15"/>
+      <c r="AK109" s="15"/>
+      <c r="AL109" s="15"/>
+      <c r="AM109" s="15"/>
+      <c r="AN109" s="15"/>
+      <c r="AO109" s="15"/>
+      <c r="AP109" s="17"/>
+    </row>
+    <row r="110" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="AG110" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH110" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI110" s="15"/>
+      <c r="AJ110" s="15"/>
+      <c r="AK110" s="15"/>
+      <c r="AL110" s="15"/>
+      <c r="AM110" s="15"/>
+      <c r="AN110" s="15"/>
+      <c r="AO110" s="15"/>
+      <c r="AP110" s="17"/>
+    </row>
+    <row r="111" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="AG111" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH111" s="39">
+        <v>1</v>
+      </c>
+      <c r="AI111" s="15"/>
+      <c r="AJ111" s="15"/>
+      <c r="AK111" s="15"/>
+      <c r="AL111" s="15"/>
+      <c r="AM111" s="15"/>
+      <c r="AN111" s="15"/>
+      <c r="AO111" s="15"/>
+      <c r="AP111" s="17"/>
+    </row>
+    <row r="112" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="AG112" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH112" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI112" s="15"/>
+      <c r="AJ112" s="15"/>
+      <c r="AK112" s="15"/>
+      <c r="AL112" s="15"/>
+      <c r="AM112" s="15"/>
+      <c r="AN112" s="15"/>
+      <c r="AO112" s="15"/>
+      <c r="AP112" s="17"/>
+    </row>
+    <row r="113" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AG113" s="18"/>
+      <c r="AH113" s="19"/>
+      <c r="AI113" s="19"/>
+      <c r="AJ113" s="19"/>
+      <c r="AK113" s="19"/>
+      <c r="AL113" s="19"/>
+      <c r="AM113" s="19"/>
+      <c r="AN113" s="19"/>
+      <c r="AO113" s="19"/>
+      <c r="AP113" s="21"/>
+    </row>
+    <row r="115" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C115" s="85"/>
+    </row>
+    <row r="116" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C116" s="87"/>
+      <c r="D116" s="16"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="16"/>
+      <c r="G116" s="16"/>
+      <c r="H116" s="16"/>
+      <c r="I116" s="16"/>
+      <c r="J116" s="16"/>
+      <c r="K116" s="16"/>
+      <c r="L116" s="16"/>
+      <c r="M116" s="16"/>
+      <c r="N116" s="16"/>
+      <c r="O116" s="16"/>
+      <c r="P116" s="16"/>
+      <c r="Q116" s="16"/>
+      <c r="R116" s="16"/>
+      <c r="S116" s="16"/>
+      <c r="T116" s="16"/>
+      <c r="U116" s="16"/>
+      <c r="V116" s="16"/>
+      <c r="W116" s="16"/>
+      <c r="X116" s="16"/>
+      <c r="Y116" s="16"/>
+      <c r="Z116" s="16"/>
+      <c r="AA116" s="16"/>
+      <c r="AB116" s="16"/>
+      <c r="AC116" s="22"/>
+    </row>
+    <row r="117" spans="3:42" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C117" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="D117" s="15"/>
+      <c r="E117" s="15"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="15"/>
+      <c r="H117" s="15"/>
+      <c r="I117" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="J117" s="15"/>
+      <c r="K117" s="15"/>
+      <c r="L117" s="15"/>
+      <c r="M117" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="N117" s="15"/>
+      <c r="O117" s="15"/>
+      <c r="P117" s="15"/>
+      <c r="Q117" s="15"/>
+      <c r="R117" s="15"/>
+      <c r="S117" s="15"/>
+      <c r="T117" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="U117" s="15"/>
+      <c r="V117" s="15"/>
+      <c r="W117" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="X117" s="15"/>
+      <c r="Y117" s="15"/>
+      <c r="Z117" s="15"/>
+      <c r="AA117" s="15"/>
+      <c r="AB117" s="15"/>
+      <c r="AC117" s="17"/>
+      <c r="AG117" s="99" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH117" s="16"/>
+      <c r="AI117" s="16"/>
+      <c r="AJ117" s="16"/>
+      <c r="AK117" s="16"/>
+      <c r="AL117" s="16"/>
+      <c r="AM117" s="16"/>
+      <c r="AN117" s="16"/>
+      <c r="AO117" s="100" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP117" s="22"/>
+    </row>
+    <row r="118" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C118" s="89"/>
+      <c r="D118" s="15"/>
+      <c r="E118" s="15"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="15"/>
+      <c r="H118" s="15"/>
+      <c r="I118" s="15"/>
+      <c r="J118" s="15"/>
+      <c r="K118" s="15"/>
+      <c r="L118" s="15"/>
+      <c r="M118" s="48"/>
+      <c r="N118" s="15"/>
+      <c r="O118" s="15"/>
+      <c r="P118" s="15"/>
+      <c r="Q118" s="15"/>
+      <c r="R118" s="15"/>
+      <c r="S118" s="15"/>
+      <c r="T118" s="15"/>
+      <c r="U118" s="15"/>
+      <c r="V118" s="15"/>
+      <c r="W118" s="48"/>
+      <c r="X118" s="15"/>
+      <c r="Y118" s="15"/>
+      <c r="Z118" s="15"/>
+      <c r="AA118" s="15"/>
+      <c r="AB118" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC118" s="17"/>
+      <c r="AG118" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH118" s="15"/>
+      <c r="AI118" s="15"/>
+      <c r="AJ118" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK118" s="15"/>
+      <c r="AL118" s="15"/>
+      <c r="AM118" s="15"/>
+      <c r="AN118" s="15"/>
+      <c r="AO118" s="15"/>
+      <c r="AP118" s="17"/>
+    </row>
+    <row r="119" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C119" s="89"/>
+      <c r="D119" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E119" s="36">
+        <v>30</v>
+      </c>
+      <c r="F119" s="15"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+      <c r="I119" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="J119" s="39">
+        <v>200</v>
+      </c>
+      <c r="K119" s="15"/>
+      <c r="L119" s="15"/>
+      <c r="M119" s="48"/>
+      <c r="N119" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="O119" s="36">
+        <v>30</v>
+      </c>
+      <c r="P119" s="15"/>
+      <c r="Q119" s="15"/>
+      <c r="R119" s="15"/>
+      <c r="S119" s="15"/>
+      <c r="T119" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="U119" s="39">
+        <v>200</v>
+      </c>
+      <c r="V119" s="15"/>
+      <c r="W119" s="48"/>
+      <c r="X119" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y119" s="36">
+        <v>30</v>
+      </c>
+      <c r="Z119" s="15"/>
+      <c r="AA119" s="15"/>
+      <c r="AB119" s="15"/>
+      <c r="AC119" s="17"/>
+      <c r="AG119" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH119" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI119" s="15"/>
+      <c r="AJ119" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK119" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL119" s="15"/>
+      <c r="AM119" s="15"/>
+      <c r="AN119" s="15"/>
+      <c r="AO119" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP119" s="90" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="120" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C120" s="89"/>
+      <c r="D120" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E120" s="36">
+        <v>30</v>
+      </c>
+      <c r="F120" s="15"/>
+      <c r="G120" s="15"/>
+      <c r="H120" s="15"/>
+      <c r="I120" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="J120" s="39">
+        <v>2</v>
+      </c>
+      <c r="K120" s="15"/>
+      <c r="L120" s="15"/>
+      <c r="M120" s="48"/>
+      <c r="N120" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="O120" s="36">
+        <v>30</v>
+      </c>
+      <c r="P120" s="15"/>
+      <c r="Q120" s="15"/>
+      <c r="R120" s="15"/>
+      <c r="S120" s="15"/>
+      <c r="T120" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="U120" s="39">
+        <v>2</v>
+      </c>
+      <c r="V120" s="15"/>
+      <c r="W120" s="48"/>
+      <c r="X120" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y120" s="36">
+        <v>30</v>
+      </c>
+      <c r="Z120" s="15"/>
+      <c r="AA120" s="15"/>
+      <c r="AB120" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC120" s="90">
+        <v>200</v>
+      </c>
+      <c r="AG120" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH120" s="39">
+        <v>8</v>
+      </c>
+      <c r="AI120" s="15"/>
+      <c r="AJ120" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK120" s="39">
+        <v>4</v>
+      </c>
+      <c r="AL120" s="15"/>
+      <c r="AM120" s="15"/>
+      <c r="AN120" s="15"/>
+      <c r="AO120" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP120" s="90" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="121" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C121" s="89"/>
+      <c r="D121" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E121" s="37">
+        <v>0.8</v>
+      </c>
+      <c r="F121" s="15"/>
+      <c r="G121" s="15"/>
+      <c r="H121" s="15"/>
+      <c r="I121" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="J121" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="K121" s="15"/>
+      <c r="L121" s="15"/>
+      <c r="M121" s="48"/>
+      <c r="N121" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="O121" s="37">
+        <v>0.875</v>
+      </c>
+      <c r="P121" s="15"/>
+      <c r="Q121" s="15"/>
+      <c r="R121" s="15"/>
+      <c r="S121" s="15"/>
+      <c r="T121" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="U121" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="V121" s="15"/>
+      <c r="W121" s="48"/>
+      <c r="X121" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y121" s="37">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="Z121" s="15"/>
+      <c r="AA121" s="15"/>
+      <c r="AB121" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC121" s="90">
+        <v>2</v>
+      </c>
+      <c r="AG121" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH121" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI121" s="15"/>
+      <c r="AJ121" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK121" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL121" s="15"/>
+      <c r="AM121" s="15"/>
+      <c r="AN121" s="15"/>
+      <c r="AO121" s="15"/>
+      <c r="AP121" s="17"/>
+    </row>
+    <row r="122" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C122" s="89"/>
+      <c r="D122" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E122" s="37">
+        <v>0.57140000000000002</v>
+      </c>
+      <c r="F122" s="15"/>
+      <c r="G122" s="15"/>
+      <c r="H122" s="15"/>
+      <c r="I122" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="J122" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K122" s="15"/>
+      <c r="L122" s="15"/>
+      <c r="M122" s="48"/>
+      <c r="N122" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O122" s="37">
+        <v>0.58330000000000004</v>
+      </c>
+      <c r="P122" s="15"/>
+      <c r="Q122" s="15"/>
+      <c r="R122" s="15"/>
+      <c r="S122" s="15"/>
+      <c r="T122" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="U122" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="V122" s="15"/>
+      <c r="W122" s="48"/>
+      <c r="X122" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y122" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="Z122" s="15"/>
+      <c r="AA122" s="15"/>
+      <c r="AB122" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC122" s="90">
+        <v>0.3</v>
+      </c>
+      <c r="AG122" s="89"/>
+      <c r="AH122" s="15"/>
+      <c r="AI122" s="15"/>
+      <c r="AJ122" s="15"/>
+      <c r="AK122" s="15"/>
+      <c r="AL122" s="15"/>
+      <c r="AM122" s="15"/>
+      <c r="AN122" s="15"/>
+      <c r="AO122" s="15"/>
+      <c r="AP122" s="17"/>
+    </row>
+    <row r="123" spans="3:42" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C123" s="89"/>
+      <c r="D123" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="E123" s="84">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="F123" s="15"/>
+      <c r="G123" s="15"/>
+      <c r="H123" s="15"/>
+      <c r="I123" s="15"/>
+      <c r="J123" s="15"/>
+      <c r="K123" s="15"/>
+      <c r="L123" s="15"/>
+      <c r="M123" s="48"/>
+      <c r="N123" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="O123" s="84">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="P123" s="15"/>
+      <c r="Q123" s="15"/>
+      <c r="R123" s="15"/>
+      <c r="S123" s="15"/>
+      <c r="T123" s="86" t="s">
+        <v>101</v>
+      </c>
+      <c r="U123" s="86">
+        <v>1E-3</v>
+      </c>
+      <c r="V123" s="15"/>
+      <c r="W123" s="48"/>
+      <c r="X123" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y123" s="84">
+        <v>0.38890000000000002</v>
+      </c>
+      <c r="Z123" s="15"/>
+      <c r="AA123" s="15"/>
+      <c r="AB123" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC123" s="90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD123" s="15"/>
+      <c r="AE123" s="15"/>
+      <c r="AG123" s="95" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH123" s="15"/>
+      <c r="AI123" s="15"/>
+      <c r="AJ123" s="15"/>
+      <c r="AK123" s="15"/>
+      <c r="AL123" s="15"/>
+      <c r="AM123" s="15"/>
+      <c r="AN123" s="15"/>
+      <c r="AO123" s="15"/>
+      <c r="AP123" s="17"/>
+    </row>
+    <row r="124" spans="3:42" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C124" s="89"/>
+      <c r="D124" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="E124" s="84">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="F124" s="15"/>
+      <c r="G124" s="15"/>
+      <c r="H124" s="15"/>
+      <c r="I124" s="15"/>
+      <c r="J124" s="15"/>
+      <c r="K124" s="15"/>
+      <c r="L124" s="15"/>
+      <c r="M124" s="48"/>
+      <c r="N124" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="O124" s="84">
+        <v>0.625</v>
+      </c>
+      <c r="P124" s="15"/>
+      <c r="Q124" s="15"/>
+      <c r="R124" s="15"/>
+      <c r="S124" s="15"/>
+      <c r="T124" s="15"/>
+      <c r="U124" s="15"/>
+      <c r="V124" s="15"/>
+      <c r="W124" s="48"/>
+      <c r="X124" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y124" s="84">
+        <v>0.37659999999999999</v>
+      </c>
+      <c r="Z124" s="15"/>
+      <c r="AA124" s="15"/>
+      <c r="AB124" s="86" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC124" s="93">
+        <v>0.01</v>
+      </c>
+      <c r="AG124" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH124" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI124" s="15"/>
+      <c r="AJ124" s="15"/>
+      <c r="AK124" s="15"/>
+      <c r="AL124" s="15"/>
+      <c r="AM124" s="15"/>
+      <c r="AN124" s="15"/>
+      <c r="AO124" s="15"/>
+      <c r="AP124" s="17"/>
+    </row>
+    <row r="125" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C125" s="89"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="15"/>
+      <c r="H125" s="15"/>
+      <c r="I125" s="15"/>
+      <c r="J125" s="15"/>
+      <c r="K125" s="15"/>
+      <c r="L125" s="15"/>
+      <c r="M125" s="15"/>
+      <c r="N125" s="15"/>
+      <c r="O125" s="15"/>
+      <c r="P125" s="15"/>
+      <c r="Q125" s="15"/>
+      <c r="R125" s="15"/>
+      <c r="S125" s="15"/>
+      <c r="T125" s="15"/>
+      <c r="U125" s="15"/>
+      <c r="V125" s="15"/>
+      <c r="W125" s="15"/>
+      <c r="X125" s="15"/>
+      <c r="Y125" s="15"/>
+      <c r="Z125" s="15"/>
+      <c r="AA125" s="15"/>
+      <c r="AB125" s="15"/>
+      <c r="AC125" s="17"/>
+      <c r="AG125" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH125" s="39">
+        <v>1</v>
+      </c>
+      <c r="AI125" s="15"/>
+      <c r="AJ125" s="15"/>
+      <c r="AK125" s="15"/>
+      <c r="AL125" s="15"/>
+      <c r="AM125" s="15"/>
+      <c r="AN125" s="15"/>
+      <c r="AO125" s="15"/>
+      <c r="AP125" s="17"/>
+    </row>
+    <row r="126" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C126" s="91"/>
+      <c r="D126" s="50"/>
+      <c r="E126" s="50"/>
+      <c r="F126" s="50"/>
+      <c r="G126" s="50"/>
+      <c r="H126" s="15"/>
+      <c r="I126" s="15"/>
+      <c r="J126" s="15"/>
+      <c r="K126" s="15"/>
+      <c r="L126" s="15"/>
+      <c r="M126" s="15"/>
+      <c r="N126" s="15"/>
+      <c r="O126" s="15"/>
+      <c r="P126" s="15"/>
+      <c r="Q126" s="15"/>
+      <c r="R126" s="15"/>
+      <c r="S126" s="15"/>
+      <c r="T126" s="15"/>
+      <c r="U126" s="15"/>
+      <c r="V126" s="15"/>
+      <c r="W126" s="15"/>
+      <c r="X126" s="15"/>
+      <c r="Y126" s="15"/>
+      <c r="Z126" s="15"/>
+      <c r="AA126" s="15"/>
+      <c r="AB126" s="15"/>
+      <c r="AC126" s="17"/>
+      <c r="AG126" s="97" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH126" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI126" s="50"/>
+      <c r="AJ126" s="50"/>
+      <c r="AK126" s="50"/>
+      <c r="AL126" s="15"/>
+      <c r="AM126" s="15"/>
+      <c r="AN126" s="15"/>
+      <c r="AO126" s="15"/>
+      <c r="AP126" s="17"/>
+    </row>
+    <row r="127" spans="3:42" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C127" s="92" t="s">
+        <v>92</v>
+      </c>
+      <c r="D127" s="59"/>
+      <c r="E127" s="59"/>
+      <c r="F127" s="59"/>
+      <c r="G127" s="59"/>
+      <c r="H127" s="15"/>
+      <c r="I127" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="J127" s="15"/>
+      <c r="K127" s="15"/>
+      <c r="L127" s="15"/>
+      <c r="M127" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="N127" s="59"/>
+      <c r="O127" s="59"/>
+      <c r="P127" s="59"/>
+      <c r="Q127" s="59"/>
+      <c r="R127" s="15"/>
+      <c r="S127" s="15"/>
+      <c r="T127" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="U127" s="15"/>
+      <c r="V127" s="15"/>
+      <c r="W127" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="X127" s="59"/>
+      <c r="Y127" s="59"/>
+      <c r="Z127" s="59"/>
+      <c r="AA127" s="59"/>
+      <c r="AB127" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC127" s="17"/>
+      <c r="AG127" s="89"/>
+      <c r="AH127" s="15"/>
+      <c r="AI127" s="15"/>
+      <c r="AJ127" s="15"/>
+      <c r="AK127" s="15"/>
+      <c r="AL127" s="15"/>
+      <c r="AM127" s="15"/>
+      <c r="AN127" s="15"/>
+      <c r="AO127" s="15"/>
+      <c r="AP127" s="17"/>
+    </row>
+    <row r="128" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C128" s="89"/>
+      <c r="D128" s="15"/>
+      <c r="E128" s="15"/>
+      <c r="F128" s="15"/>
+      <c r="G128" s="15"/>
+      <c r="H128" s="15"/>
+      <c r="I128" s="15"/>
+      <c r="J128" s="15"/>
+      <c r="K128" s="15"/>
+      <c r="L128" s="15"/>
+      <c r="M128" s="48"/>
+      <c r="N128" s="15"/>
+      <c r="O128" s="15"/>
+      <c r="P128" s="15"/>
+      <c r="Q128" s="15"/>
+      <c r="R128" s="15"/>
+      <c r="S128" s="15"/>
+      <c r="T128" s="15"/>
+      <c r="U128" s="15"/>
+      <c r="V128" s="15"/>
+      <c r="W128" s="48"/>
+      <c r="X128" s="15"/>
+      <c r="Y128" s="15"/>
+      <c r="Z128" s="15"/>
+      <c r="AA128" s="15"/>
+      <c r="AB128" s="15"/>
+      <c r="AC128" s="17"/>
+      <c r="AG128" s="89"/>
+      <c r="AH128" s="15"/>
+      <c r="AI128" s="15"/>
+      <c r="AJ128" s="15"/>
+      <c r="AK128" s="15"/>
+      <c r="AL128" s="15"/>
+      <c r="AM128" s="15"/>
+      <c r="AN128" s="15"/>
+      <c r="AO128" s="15"/>
+      <c r="AP128" s="17"/>
+    </row>
+    <row r="129" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C129" s="89"/>
+      <c r="D129" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E129" s="36">
+        <v>30</v>
+      </c>
+      <c r="F129" s="15"/>
+      <c r="G129" s="15"/>
+      <c r="H129" s="15"/>
+      <c r="I129" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="J129" s="39">
+        <v>20</v>
+      </c>
+      <c r="K129" s="15"/>
+      <c r="L129" s="15"/>
+      <c r="M129" s="48"/>
+      <c r="N129" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="O129" s="36">
+        <v>30</v>
+      </c>
+      <c r="P129" s="15"/>
+      <c r="Q129" s="15"/>
+      <c r="R129" s="15"/>
+      <c r="S129" s="15"/>
+      <c r="T129" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="U129" s="39">
+        <v>10</v>
+      </c>
+      <c r="V129" s="15"/>
+      <c r="W129" s="48"/>
+      <c r="X129" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y129" s="36">
+        <v>30</v>
+      </c>
+      <c r="Z129" s="15"/>
+      <c r="AA129" s="15"/>
+      <c r="AB129" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC129" s="90">
+        <v>100</v>
+      </c>
+      <c r="AG129" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH129" s="15"/>
+      <c r="AI129" s="15"/>
+      <c r="AJ129" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK129" s="15"/>
+      <c r="AL129" s="15"/>
+      <c r="AM129" s="15"/>
+      <c r="AN129" s="15"/>
+      <c r="AO129" s="15"/>
+      <c r="AP129" s="17"/>
+    </row>
+    <row r="130" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C130" s="89"/>
+      <c r="D130" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E130" s="36">
+        <v>30</v>
+      </c>
+      <c r="F130" s="15"/>
+      <c r="G130" s="15"/>
+      <c r="H130" s="15"/>
+      <c r="I130" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="J130" s="39">
+        <v>2</v>
+      </c>
+      <c r="K130" s="15"/>
+      <c r="L130" s="15"/>
+      <c r="M130" s="48"/>
+      <c r="N130" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="O130" s="36">
+        <v>30</v>
+      </c>
+      <c r="P130" s="15"/>
+      <c r="Q130" s="15"/>
+      <c r="R130" s="15"/>
+      <c r="S130" s="15"/>
+      <c r="T130" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="U130" s="39">
+        <v>2</v>
+      </c>
+      <c r="V130" s="15"/>
+      <c r="W130" s="48"/>
+      <c r="X130" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y130" s="36">
+        <v>30</v>
+      </c>
+      <c r="Z130" s="15"/>
+      <c r="AA130" s="15"/>
+      <c r="AB130" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC130" s="90">
+        <v>2</v>
+      </c>
+      <c r="AG130" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH130" s="15"/>
+      <c r="AI130" s="15"/>
+      <c r="AJ130" s="15"/>
+      <c r="AK130" s="15"/>
+      <c r="AL130" s="15"/>
+      <c r="AM130" s="15"/>
+      <c r="AN130" s="15"/>
+      <c r="AO130" s="15"/>
+      <c r="AP130" s="17"/>
+    </row>
+    <row r="131" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C131" s="89"/>
+      <c r="D131" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E131" s="37">
+        <v>0.7</v>
+      </c>
+      <c r="F131" s="15"/>
+      <c r="G131" s="15"/>
+      <c r="H131" s="15"/>
+      <c r="I131" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="J131" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="K131" s="15"/>
+      <c r="L131" s="15"/>
+      <c r="M131" s="48"/>
+      <c r="N131" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="O131" s="37">
+        <v>1</v>
+      </c>
+      <c r="P131" s="15"/>
+      <c r="Q131" s="15"/>
+      <c r="R131" s="15"/>
+      <c r="S131" s="15"/>
+      <c r="T131" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="U131" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="V131" s="15"/>
+      <c r="W131" s="48"/>
+      <c r="X131" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y131" s="37">
+        <v>0.2727</v>
+      </c>
+      <c r="Z131" s="15"/>
+      <c r="AA131" s="15"/>
+      <c r="AB131" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC131" s="90">
+        <v>0.3</v>
+      </c>
+      <c r="AG131" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH131" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI131" s="15"/>
+      <c r="AJ131" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK131" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL131" s="15"/>
+      <c r="AM131" s="15"/>
+      <c r="AN131" s="15"/>
+      <c r="AO131" s="15"/>
+      <c r="AP131" s="17"/>
+    </row>
+    <row r="132" spans="3:42" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C132" s="89"/>
+      <c r="D132" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E132" s="37">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="F132" s="15"/>
+      <c r="G132" s="15"/>
+      <c r="H132" s="15"/>
+      <c r="I132" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="J132" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K132" s="15"/>
+      <c r="L132" s="15"/>
+      <c r="M132" s="48"/>
+      <c r="N132" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O132" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="P132" s="15"/>
+      <c r="Q132" s="15"/>
+      <c r="R132" s="15"/>
+      <c r="S132" s="15"/>
+      <c r="T132" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="U132" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="V132" s="15"/>
+      <c r="W132" s="48"/>
+      <c r="X132" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y132" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="Z132" s="15"/>
+      <c r="AA132" s="15"/>
+      <c r="AB132" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC132" s="90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG132" s="96" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH132" s="39">
+        <v>16</v>
+      </c>
+      <c r="AI132" s="15"/>
+      <c r="AJ132" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK132" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL132" s="15"/>
+      <c r="AM132" s="15"/>
+      <c r="AN132" s="15"/>
+      <c r="AO132" s="15"/>
+      <c r="AP132" s="17"/>
+    </row>
+    <row r="133" spans="3:42" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C133" s="89"/>
+      <c r="D133" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="E133" s="84">
+        <v>0.61109999999999998</v>
+      </c>
+      <c r="F133" s="15"/>
+      <c r="G133" s="15"/>
+      <c r="H133" s="15"/>
+      <c r="I133" s="86" t="s">
+        <v>101</v>
+      </c>
+      <c r="J133" s="86">
+        <v>1E-4</v>
+      </c>
+      <c r="K133" s="15"/>
+      <c r="L133" s="15"/>
+      <c r="M133" s="48"/>
+      <c r="N133" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="O133" s="84">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="P133" s="15"/>
+      <c r="Q133" s="15"/>
+      <c r="R133" s="15"/>
+      <c r="S133" s="15"/>
+      <c r="T133" s="86" t="s">
+        <v>101</v>
+      </c>
+      <c r="U133" s="86">
+        <v>1E-4</v>
+      </c>
+      <c r="V133" s="15"/>
+      <c r="W133" s="48"/>
+      <c r="X133" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y133" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="Z133" s="15"/>
+      <c r="AA133" s="15"/>
+      <c r="AB133" s="15"/>
+      <c r="AC133" s="17"/>
+      <c r="AG133" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH133" s="39">
+        <v>3</v>
+      </c>
+      <c r="AI133" s="15"/>
+      <c r="AJ133" s="15"/>
+      <c r="AK133" s="15"/>
+      <c r="AL133" s="15"/>
+      <c r="AM133" s="15"/>
+      <c r="AN133" s="15"/>
+      <c r="AO133" s="15"/>
+      <c r="AP133" s="17"/>
+    </row>
+    <row r="134" spans="3:42" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C134" s="89"/>
+      <c r="D134" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="E134" s="84">
+        <v>0.49380000000000002</v>
+      </c>
+      <c r="F134" s="15"/>
+      <c r="G134" s="15"/>
+      <c r="H134" s="15"/>
+      <c r="I134" s="15"/>
+      <c r="J134" s="15"/>
+      <c r="K134" s="15"/>
+      <c r="L134" s="15"/>
+      <c r="M134" s="48"/>
+      <c r="N134" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="O134" s="84">
+        <v>0.55620000000000003</v>
+      </c>
+      <c r="P134" s="15"/>
+      <c r="Q134" s="15"/>
+      <c r="R134" s="15"/>
+      <c r="S134" s="15"/>
+      <c r="T134" s="15"/>
+      <c r="U134" s="15"/>
+      <c r="V134" s="15"/>
+      <c r="W134" s="48"/>
+      <c r="X134" s="83" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y134" s="84">
+        <v>0.62339999999999995</v>
+      </c>
+      <c r="Z134" s="15"/>
+      <c r="AA134" s="15"/>
+      <c r="AB134" s="15"/>
+      <c r="AC134" s="17"/>
+      <c r="AG134" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH134" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI134" s="15"/>
+      <c r="AJ134" s="15"/>
+      <c r="AK134" s="15"/>
+      <c r="AL134" s="15"/>
+      <c r="AM134" s="15"/>
+      <c r="AN134" s="15"/>
+      <c r="AO134" s="15"/>
+      <c r="AP134" s="17"/>
+    </row>
+    <row r="135" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C135" s="89"/>
+      <c r="D135" s="15"/>
+      <c r="E135" s="15"/>
+      <c r="F135" s="15"/>
+      <c r="G135" s="15"/>
+      <c r="H135" s="15"/>
+      <c r="I135" s="15"/>
+      <c r="J135" s="15"/>
+      <c r="K135" s="15"/>
+      <c r="L135" s="15"/>
+      <c r="M135" s="48"/>
+      <c r="N135" s="15"/>
+      <c r="O135" s="15"/>
+      <c r="P135" s="15"/>
+      <c r="Q135" s="15"/>
+      <c r="R135" s="15"/>
+      <c r="S135" s="15"/>
+      <c r="T135" s="15"/>
+      <c r="U135" s="15"/>
+      <c r="V135" s="15"/>
+      <c r="W135" s="48"/>
+      <c r="X135" s="15"/>
+      <c r="Y135" s="15"/>
+      <c r="Z135" s="15"/>
+      <c r="AA135" s="15"/>
+      <c r="AB135" s="15"/>
+      <c r="AC135" s="17"/>
+      <c r="AG135" s="89"/>
+      <c r="AH135" s="15"/>
+      <c r="AI135" s="15"/>
+      <c r="AJ135" s="15"/>
+      <c r="AK135" s="15"/>
+      <c r="AL135" s="15"/>
+      <c r="AM135" s="15"/>
+      <c r="AN135" s="15"/>
+      <c r="AO135" s="15"/>
+      <c r="AP135" s="17"/>
+    </row>
+    <row r="136" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C136" s="89"/>
+      <c r="D136" s="15"/>
+      <c r="E136" s="15"/>
+      <c r="F136" s="15"/>
+      <c r="G136" s="15"/>
+      <c r="H136" s="15"/>
+      <c r="I136" s="15"/>
+      <c r="J136" s="15"/>
+      <c r="K136" s="15"/>
+      <c r="L136" s="15"/>
+      <c r="M136" s="15"/>
+      <c r="N136" s="15"/>
+      <c r="O136" s="15"/>
+      <c r="P136" s="15"/>
+      <c r="Q136" s="15"/>
+      <c r="R136" s="15"/>
+      <c r="S136" s="15"/>
+      <c r="T136" s="15"/>
+      <c r="U136" s="15"/>
+      <c r="V136" s="15"/>
+      <c r="W136" s="15"/>
+      <c r="X136" s="15"/>
+      <c r="Y136" s="15"/>
+      <c r="Z136" s="15"/>
+      <c r="AA136" s="15"/>
+      <c r="AB136" s="15"/>
+      <c r="AC136" s="17"/>
+      <c r="AG136" s="95" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH136" s="15"/>
+      <c r="AI136" s="15"/>
+      <c r="AJ136" s="15"/>
+      <c r="AK136" s="15"/>
+      <c r="AL136" s="15"/>
+      <c r="AM136" s="15"/>
+      <c r="AN136" s="15"/>
+      <c r="AO136" s="15"/>
+      <c r="AP136" s="17"/>
+    </row>
+    <row r="137" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C137" s="89"/>
+      <c r="D137" s="15"/>
+      <c r="E137" s="15"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="15"/>
+      <c r="H137" s="15"/>
+      <c r="I137" s="15"/>
+      <c r="J137" s="15"/>
+      <c r="K137" s="15"/>
+      <c r="L137" s="15"/>
+      <c r="M137" s="15"/>
+      <c r="N137" s="15"/>
+      <c r="O137" s="15"/>
+      <c r="P137" s="15"/>
+      <c r="Q137" s="15"/>
+      <c r="R137" s="15"/>
+      <c r="S137" s="15"/>
+      <c r="T137" s="15"/>
+      <c r="U137" s="15"/>
+      <c r="V137" s="15"/>
+      <c r="W137" s="15"/>
+      <c r="X137" s="15"/>
+      <c r="Y137" s="15"/>
+      <c r="Z137" s="15"/>
+      <c r="AA137" s="15"/>
+      <c r="AB137" s="15"/>
+      <c r="AC137" s="17"/>
+      <c r="AG137" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH137" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI137" s="15"/>
+      <c r="AJ137" s="15"/>
+      <c r="AK137" s="15"/>
+      <c r="AL137" s="15"/>
+      <c r="AM137" s="15"/>
+      <c r="AN137" s="15"/>
+      <c r="AO137" s="15"/>
+      <c r="AP137" s="17"/>
+    </row>
+    <row r="138" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C138" s="89"/>
+      <c r="D138" s="15"/>
+      <c r="E138" s="15"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="15"/>
+      <c r="H138" s="15"/>
+      <c r="I138" s="15"/>
+      <c r="J138" s="15"/>
+      <c r="K138" s="15"/>
+      <c r="L138" s="15"/>
+      <c r="M138" s="15"/>
+      <c r="N138" s="15"/>
+      <c r="O138" s="15"/>
+      <c r="P138" s="15"/>
+      <c r="Q138" s="15"/>
+      <c r="R138" s="15"/>
+      <c r="S138" s="15"/>
+      <c r="T138" s="15"/>
+      <c r="U138" s="15"/>
+      <c r="V138" s="15"/>
+      <c r="W138" s="15"/>
+      <c r="X138" s="15"/>
+      <c r="Y138" s="15"/>
+      <c r="Z138" s="15"/>
+      <c r="AA138" s="15"/>
+      <c r="AB138" s="15"/>
+      <c r="AC138" s="17"/>
+      <c r="AG138" s="96" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH138" s="39">
+        <v>8</v>
+      </c>
+      <c r="AI138" s="15"/>
+      <c r="AJ138" s="15"/>
+      <c r="AK138" s="15"/>
+      <c r="AL138" s="15"/>
+      <c r="AM138" s="15"/>
+      <c r="AN138" s="15"/>
+      <c r="AO138" s="15"/>
+      <c r="AP138" s="17"/>
+    </row>
+    <row r="139" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C139" s="89"/>
+      <c r="D139" s="15"/>
+      <c r="E139" s="15"/>
+      <c r="F139" s="15"/>
+      <c r="G139" s="15"/>
+      <c r="H139" s="15"/>
+      <c r="I139" s="15"/>
+      <c r="J139" s="15"/>
+      <c r="K139" s="15"/>
+      <c r="L139" s="15"/>
+      <c r="M139" s="15"/>
+      <c r="N139" s="15"/>
+      <c r="O139" s="15"/>
+      <c r="P139" s="15"/>
+      <c r="Q139" s="15"/>
+      <c r="R139" s="15"/>
+      <c r="S139" s="15"/>
+      <c r="T139" s="15"/>
+      <c r="U139" s="15"/>
+      <c r="V139" s="15"/>
+      <c r="W139" s="15"/>
+      <c r="X139" s="15"/>
+      <c r="Y139" s="15"/>
+      <c r="Z139" s="15"/>
+      <c r="AA139" s="15"/>
+      <c r="AB139" s="15"/>
+      <c r="AC139" s="17"/>
+      <c r="AG139" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH139" s="39">
+        <v>3</v>
+      </c>
+      <c r="AI139" s="15"/>
+      <c r="AJ139" s="15"/>
+      <c r="AK139" s="15"/>
+      <c r="AL139" s="15"/>
+      <c r="AM139" s="15"/>
+      <c r="AN139" s="15"/>
+      <c r="AO139" s="15"/>
+      <c r="AP139" s="17"/>
+    </row>
+    <row r="140" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="C140" s="89"/>
+      <c r="D140" s="15"/>
+      <c r="E140" s="15"/>
+      <c r="F140" s="15"/>
+      <c r="G140" s="15"/>
+      <c r="H140" s="15"/>
+      <c r="I140" s="15"/>
+      <c r="J140" s="15"/>
+      <c r="K140" s="15"/>
+      <c r="L140" s="15"/>
+      <c r="M140" s="15"/>
+      <c r="N140" s="15"/>
+      <c r="O140" s="15"/>
+      <c r="P140" s="15"/>
+      <c r="Q140" s="15"/>
+      <c r="R140" s="15"/>
+      <c r="S140" s="15"/>
+      <c r="T140" s="15"/>
+      <c r="U140" s="15"/>
+      <c r="V140" s="15"/>
+      <c r="W140" s="15"/>
+      <c r="X140" s="15"/>
+      <c r="Y140" s="15"/>
+      <c r="Z140" s="15"/>
+      <c r="AA140" s="15"/>
+      <c r="AB140" s="15"/>
+      <c r="AC140" s="17"/>
+      <c r="AG140" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH140" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI140" s="15"/>
+      <c r="AJ140" s="15"/>
+      <c r="AK140" s="15"/>
+      <c r="AL140" s="15"/>
+      <c r="AM140" s="15"/>
+      <c r="AN140" s="15"/>
+      <c r="AO140" s="15"/>
+      <c r="AP140" s="17"/>
+    </row>
+    <row r="141" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C141" s="18"/>
+      <c r="D141" s="19"/>
+      <c r="E141" s="19"/>
+      <c r="F141" s="19"/>
+      <c r="G141" s="19"/>
+      <c r="H141" s="19"/>
+      <c r="I141" s="19"/>
+      <c r="J141" s="19"/>
+      <c r="K141" s="19"/>
+      <c r="L141" s="19"/>
+      <c r="M141" s="19"/>
+      <c r="N141" s="19"/>
+      <c r="O141" s="19"/>
+      <c r="P141" s="19"/>
+      <c r="Q141" s="19"/>
+      <c r="R141" s="19"/>
+      <c r="S141" s="19"/>
+      <c r="T141" s="19"/>
+      <c r="U141" s="19"/>
+      <c r="V141" s="19"/>
+      <c r="W141" s="19"/>
+      <c r="X141" s="19"/>
+      <c r="Y141" s="19"/>
+      <c r="Z141" s="19"/>
+      <c r="AA141" s="19"/>
+      <c r="AB141" s="19"/>
+      <c r="AC141" s="21"/>
+      <c r="AG141" s="95" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH141" s="15"/>
+      <c r="AI141" s="15"/>
+      <c r="AJ141" s="15"/>
+      <c r="AK141" s="15"/>
+      <c r="AL141" s="15"/>
+      <c r="AM141" s="15"/>
+      <c r="AN141" s="15"/>
+      <c r="AO141" s="15"/>
+      <c r="AP141" s="17"/>
+    </row>
+    <row r="142" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="AG142" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH142" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI142" s="15"/>
+      <c r="AJ142" s="15"/>
+      <c r="AK142" s="15"/>
+      <c r="AL142" s="15"/>
+      <c r="AM142" s="15"/>
+      <c r="AN142" s="15"/>
+      <c r="AO142" s="15"/>
+      <c r="AP142" s="17"/>
+    </row>
+    <row r="143" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="AG143" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH143" s="39">
+        <v>1</v>
+      </c>
+      <c r="AI143" s="15"/>
+      <c r="AJ143" s="15"/>
+      <c r="AK143" s="15"/>
+      <c r="AL143" s="15"/>
+      <c r="AM143" s="15"/>
+      <c r="AN143" s="15"/>
+      <c r="AO143" s="15"/>
+      <c r="AP143" s="17"/>
+    </row>
+    <row r="144" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AG144" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH144" s="102" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI144" s="19"/>
+      <c r="AJ144" s="19"/>
+      <c r="AK144" s="19"/>
+      <c r="AL144" s="19"/>
+      <c r="AM144" s="19"/>
+      <c r="AN144" s="19"/>
+      <c r="AO144" s="19"/>
+      <c r="AP144" s="21"/>
+    </row>
+    <row r="146" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="147" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C147" s="87"/>
+      <c r="D147" s="16"/>
+      <c r="E147" s="16"/>
+      <c r="F147" s="16"/>
+      <c r="G147" s="16"/>
+      <c r="H147" s="16"/>
+      <c r="I147" s="16"/>
+      <c r="J147" s="16"/>
+      <c r="K147" s="16"/>
+      <c r="L147" s="16"/>
+      <c r="M147" s="16"/>
+      <c r="N147" s="16"/>
+      <c r="O147" s="16"/>
+      <c r="P147" s="16"/>
+      <c r="Q147" s="16"/>
+      <c r="R147" s="16"/>
+      <c r="S147" s="16"/>
+      <c r="T147" s="22"/>
+    </row>
+    <row r="148" spans="3:20" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C148" s="88" t="s">
+        <v>80</v>
+      </c>
+      <c r="D148" s="15"/>
+      <c r="E148" s="15"/>
+      <c r="F148" s="15"/>
+      <c r="G148" s="15"/>
+      <c r="H148" s="15"/>
+      <c r="I148" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="J148" s="15"/>
+      <c r="K148" s="15"/>
+      <c r="L148" s="15"/>
+      <c r="M148" s="15"/>
+      <c r="N148" s="15"/>
+      <c r="O148" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="P148" s="15"/>
+      <c r="Q148" s="15"/>
+      <c r="R148" s="15"/>
+      <c r="S148" s="15"/>
+      <c r="T148" s="17"/>
+    </row>
+    <row r="149" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C149" s="89"/>
+      <c r="D149" s="15"/>
+      <c r="E149" s="15"/>
+      <c r="F149" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G149" s="15"/>
+      <c r="H149" s="15"/>
+      <c r="I149" s="15"/>
+      <c r="J149" s="15"/>
+      <c r="K149" s="15"/>
+      <c r="L149" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="M149" s="15"/>
+      <c r="N149" s="15"/>
+      <c r="O149" s="15"/>
+      <c r="P149" s="15"/>
+      <c r="Q149" s="15"/>
+      <c r="R149" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="S149" s="15"/>
+      <c r="T149" s="17"/>
+    </row>
+    <row r="150" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C150" s="89"/>
+      <c r="D150" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E150" s="36">
+        <v>25</v>
+      </c>
+      <c r="F150" s="15"/>
+      <c r="G150" s="15"/>
+      <c r="H150" s="15"/>
+      <c r="I150" s="15"/>
+      <c r="J150" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K150" s="36">
+        <v>25</v>
+      </c>
+      <c r="L150" s="15"/>
+      <c r="M150" s="15"/>
+      <c r="N150" s="15"/>
+      <c r="O150" s="15"/>
+      <c r="P150" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q150" s="36">
+        <v>25</v>
+      </c>
+      <c r="R150" s="15"/>
+      <c r="S150" s="15"/>
+      <c r="T150" s="17"/>
+    </row>
+    <row r="151" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C151" s="89"/>
+      <c r="D151" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E151" s="36">
+        <v>25</v>
+      </c>
+      <c r="F151" s="15"/>
+      <c r="G151" s="15"/>
+      <c r="H151" s="15"/>
+      <c r="I151" s="15"/>
+      <c r="J151" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="K151" s="36">
+        <v>25</v>
+      </c>
+      <c r="L151" s="15"/>
+      <c r="M151" s="15"/>
+      <c r="N151" s="15"/>
+      <c r="O151" s="15"/>
+      <c r="P151" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q151" s="36">
+        <v>25</v>
+      </c>
+      <c r="R151" s="15"/>
+      <c r="S151" s="15"/>
+      <c r="T151" s="17"/>
+    </row>
+    <row r="152" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C152" s="89"/>
+      <c r="D152" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E152" s="37">
+        <v>0.47749999999999998</v>
+      </c>
+      <c r="F152" s="44">
+        <v>0.215</v>
+      </c>
+      <c r="G152" s="15"/>
+      <c r="H152" s="15"/>
+      <c r="I152" s="15"/>
+      <c r="J152" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="K152" s="37">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="L152" s="44">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="M152" s="15"/>
+      <c r="N152" s="15"/>
+      <c r="O152" s="15"/>
+      <c r="P152" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q152" s="37">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="R152" s="44">
+        <v>0.108</v>
+      </c>
+      <c r="S152" s="15"/>
+      <c r="T152" s="17"/>
+    </row>
+    <row r="153" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C153" s="89"/>
+      <c r="D153" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E153" s="37">
+        <v>0.56289999999999996</v>
+      </c>
+      <c r="F153" s="44">
+        <v>0.129</v>
+      </c>
+      <c r="G153" s="15"/>
+      <c r="H153" s="15"/>
+      <c r="I153" s="15"/>
+      <c r="J153" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="K153" s="37">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="L153" s="44">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="M153" s="15"/>
+      <c r="N153" s="15"/>
+      <c r="O153" s="15"/>
+      <c r="P153" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q153" s="37">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="R153" s="44">
+        <v>0.113</v>
+      </c>
+      <c r="S153" s="15"/>
+      <c r="T153" s="17"/>
+    </row>
+    <row r="154" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C154" s="89"/>
+      <c r="D154" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E154" s="36">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="F154" s="44">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G154" s="15"/>
+      <c r="H154" s="15"/>
+      <c r="I154" s="15"/>
+      <c r="J154" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="K154" s="36">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="L154" s="44">
+        <v>7.8200000000000006E-2</v>
+      </c>
+      <c r="M154" s="15"/>
+      <c r="N154" s="15"/>
+      <c r="O154" s="15"/>
+      <c r="P154" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q154" s="36">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="R154" s="44">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="S154" s="15"/>
+      <c r="T154" s="17"/>
+    </row>
+    <row r="155" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C155" s="89"/>
+      <c r="D155" s="15"/>
+      <c r="E155" s="15"/>
+      <c r="F155" s="15"/>
+      <c r="G155" s="15"/>
+      <c r="H155" s="15"/>
+      <c r="I155" s="15"/>
+      <c r="J155" s="15"/>
+      <c r="K155" s="15"/>
+      <c r="L155" s="15"/>
+      <c r="M155" s="15"/>
+      <c r="N155" s="15"/>
+      <c r="O155" s="15"/>
+      <c r="P155" s="15"/>
+      <c r="Q155" s="15"/>
+      <c r="R155" s="15"/>
+      <c r="S155" s="15"/>
+      <c r="T155" s="17"/>
+    </row>
+    <row r="156" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C156" s="89"/>
+      <c r="D156" s="15"/>
+      <c r="E156" s="15"/>
+      <c r="F156" s="15"/>
+      <c r="G156" s="15"/>
+      <c r="H156" s="15"/>
+      <c r="I156" s="15"/>
+      <c r="J156" s="15"/>
+      <c r="K156" s="15"/>
+      <c r="L156" s="15"/>
+      <c r="M156" s="15"/>
+      <c r="N156" s="15"/>
+      <c r="O156" s="15"/>
+      <c r="P156" s="15"/>
+      <c r="Q156" s="15"/>
+      <c r="R156" s="15"/>
+      <c r="S156" s="15"/>
+      <c r="T156" s="17"/>
+    </row>
+    <row r="157" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C157" s="89"/>
+      <c r="D157" s="15"/>
+      <c r="E157" s="15"/>
+      <c r="F157" s="15"/>
+      <c r="G157" s="15"/>
+      <c r="H157" s="15"/>
+      <c r="I157" s="15"/>
+      <c r="J157" s="15"/>
+      <c r="K157" s="15"/>
+      <c r="L157" s="15"/>
+      <c r="M157" s="15"/>
+      <c r="N157" s="15"/>
+      <c r="O157" s="15"/>
+      <c r="P157" s="15"/>
+      <c r="Q157" s="15"/>
+      <c r="R157" s="15"/>
+      <c r="S157" s="15"/>
+      <c r="T157" s="17"/>
+    </row>
+    <row r="158" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C158" s="89"/>
+      <c r="D158" s="15"/>
+      <c r="E158" s="15"/>
+      <c r="F158" s="15"/>
+      <c r="G158" s="15"/>
+      <c r="H158" s="15"/>
+      <c r="I158" s="15"/>
+      <c r="J158" s="15"/>
+      <c r="K158" s="15"/>
+      <c r="L158" s="15"/>
+      <c r="M158" s="15"/>
+      <c r="N158" s="15"/>
+      <c r="O158" s="15"/>
+      <c r="P158" s="15"/>
+      <c r="Q158" s="15"/>
+      <c r="R158" s="15"/>
+      <c r="S158" s="15"/>
+      <c r="T158" s="17"/>
+    </row>
+    <row r="159" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C159" s="89"/>
+      <c r="D159" s="15"/>
+      <c r="E159" s="15"/>
+      <c r="F159" s="15"/>
+      <c r="G159" s="15"/>
+      <c r="H159" s="15"/>
+      <c r="I159" s="15"/>
+      <c r="J159" s="15"/>
+      <c r="K159" s="15"/>
+      <c r="L159" s="15"/>
+      <c r="M159" s="15"/>
+      <c r="N159" s="15"/>
+      <c r="O159" s="15"/>
+      <c r="P159" s="15"/>
+      <c r="Q159" s="15"/>
+      <c r="R159" s="15"/>
+      <c r="S159" s="15"/>
+      <c r="T159" s="17"/>
+    </row>
+    <row r="160" spans="3:20" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C160" s="88" t="s">
+        <v>80</v>
+      </c>
+      <c r="D160" s="15"/>
+      <c r="E160" s="15"/>
+      <c r="F160" s="15"/>
+      <c r="G160" s="15"/>
+      <c r="H160" s="15"/>
+      <c r="I160" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="J160" s="15"/>
+      <c r="K160" s="15"/>
+      <c r="L160" s="15"/>
+      <c r="M160" s="15"/>
+      <c r="N160" s="15"/>
+      <c r="O160" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="P160" s="15"/>
+      <c r="Q160" s="15"/>
+      <c r="R160" s="15"/>
+      <c r="S160" s="15"/>
+      <c r="T160" s="17"/>
+    </row>
+    <row r="161" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C161" s="89"/>
+      <c r="D161" s="15"/>
+      <c r="E161" s="15"/>
+      <c r="F161" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G161" s="15"/>
+      <c r="H161" s="15"/>
+      <c r="I161" s="15"/>
+      <c r="J161" s="15"/>
+      <c r="K161" s="15"/>
+      <c r="L161" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="M161" s="15"/>
+      <c r="N161" s="15"/>
+      <c r="O161" s="15"/>
+      <c r="P161" s="15"/>
+      <c r="Q161" s="15"/>
+      <c r="R161" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="S161" s="15"/>
+      <c r="T161" s="17"/>
+    </row>
+    <row r="162" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C162" s="89"/>
+      <c r="D162" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E162" s="36">
+        <v>30</v>
+      </c>
+      <c r="F162" s="15"/>
+      <c r="G162" s="15"/>
+      <c r="H162" s="15"/>
+      <c r="I162" s="15"/>
+      <c r="J162" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K162" s="36">
+        <v>30</v>
+      </c>
+      <c r="L162" s="15"/>
+      <c r="M162" s="15"/>
+      <c r="N162" s="15"/>
+      <c r="O162" s="15"/>
+      <c r="P162" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q162" s="36">
+        <v>30</v>
+      </c>
+      <c r="R162" s="15"/>
+      <c r="S162" s="15"/>
+      <c r="T162" s="17"/>
+    </row>
+    <row r="163" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C163" s="89"/>
+      <c r="D163" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E163" s="36">
+        <v>30</v>
+      </c>
+      <c r="F163" s="15"/>
+      <c r="G163" s="15"/>
+      <c r="H163" s="15"/>
+      <c r="I163" s="15"/>
+      <c r="J163" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="K163" s="36">
+        <v>30</v>
+      </c>
+      <c r="L163" s="15"/>
+      <c r="M163" s="15"/>
+      <c r="N163" s="15"/>
+      <c r="O163" s="15"/>
+      <c r="P163" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q163" s="36">
+        <v>30</v>
+      </c>
+      <c r="R163" s="15"/>
+      <c r="S163" s="15"/>
+      <c r="T163" s="17"/>
+    </row>
+    <row r="164" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C164" s="89"/>
+      <c r="D164" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E164" s="37">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="F164" s="44">
+        <v>0.126</v>
+      </c>
+      <c r="G164" s="15"/>
+      <c r="H164" s="15"/>
+      <c r="I164" s="15"/>
+      <c r="J164" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="K164" s="37">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="L164" s="44">
+        <v>0.183</v>
+      </c>
+      <c r="M164" s="15"/>
+      <c r="N164" s="15"/>
+      <c r="O164" s="15"/>
+      <c r="P164" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q164" s="37">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="R164" s="44">
+        <v>0.183</v>
+      </c>
+      <c r="S164" s="15"/>
+      <c r="T164" s="17"/>
+    </row>
+    <row r="165" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C165" s="89"/>
+      <c r="D165" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E165" s="37">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="F165" s="44">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G165" s="15"/>
+      <c r="H165" s="15"/>
+      <c r="I165" s="15"/>
+      <c r="J165" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="K165" s="37">
+        <v>0.497</v>
+      </c>
+      <c r="L165" s="44">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="M165" s="15"/>
+      <c r="N165" s="15"/>
+      <c r="O165" s="15"/>
+      <c r="P165" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q165" s="37">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="R165" s="44">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="S165" s="15"/>
+      <c r="T165" s="17"/>
+    </row>
+    <row r="166" spans="3:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C166" s="89"/>
+      <c r="D166" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E166" s="36">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F166" s="44">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="G166" s="15"/>
+      <c r="H166" s="15"/>
+      <c r="I166" s="15"/>
+      <c r="J166" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="K166" s="36">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="L166" s="44">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="M166" s="15"/>
+      <c r="N166" s="15"/>
+      <c r="O166" s="15"/>
+      <c r="P166" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q166" s="36">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="R166" s="44">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="S166" s="15"/>
+      <c r="T166" s="17"/>
+    </row>
+    <row r="167" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C167" s="89"/>
+      <c r="D167" s="15"/>
+      <c r="E167" s="15"/>
+      <c r="F167" s="15"/>
+      <c r="G167" s="15"/>
+      <c r="H167" s="15"/>
+      <c r="I167" s="15"/>
+      <c r="J167" s="15"/>
+      <c r="K167" s="15"/>
+      <c r="L167" s="15"/>
+      <c r="M167" s="15"/>
+      <c r="N167" s="15"/>
+      <c r="O167" s="15"/>
+      <c r="P167" s="15"/>
+      <c r="Q167" s="15"/>
+      <c r="R167" s="15"/>
+      <c r="S167" s="15"/>
+      <c r="T167" s="17"/>
+    </row>
+    <row r="168" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C168" s="89"/>
+      <c r="D168" s="15"/>
+      <c r="E168" s="15"/>
+      <c r="F168" s="15"/>
+      <c r="G168" s="15"/>
+      <c r="H168" s="15"/>
+      <c r="I168" s="15"/>
+      <c r="J168" s="15"/>
+      <c r="K168" s="15"/>
+      <c r="L168" s="15"/>
+      <c r="M168" s="15"/>
+      <c r="N168" s="15"/>
+      <c r="O168" s="15"/>
+      <c r="P168" s="15"/>
+      <c r="Q168" s="15"/>
+      <c r="R168" s="15"/>
+      <c r="S168" s="15"/>
+      <c r="T168" s="17"/>
+    </row>
+    <row r="169" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C169" s="89"/>
+      <c r="D169" s="15"/>
+      <c r="E169" s="15"/>
+      <c r="F169" s="15"/>
+      <c r="G169" s="15"/>
+      <c r="H169" s="15"/>
+      <c r="I169" s="15"/>
+      <c r="J169" s="15"/>
+      <c r="K169" s="15"/>
+      <c r="L169" s="15"/>
+      <c r="M169" s="15"/>
+      <c r="N169" s="15"/>
+      <c r="O169" s="15"/>
+      <c r="P169" s="15"/>
+      <c r="Q169" s="15"/>
+      <c r="R169" s="15"/>
+      <c r="S169" s="15"/>
+      <c r="T169" s="17"/>
+    </row>
+    <row r="170" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C170" s="89"/>
+      <c r="D170" s="15"/>
+      <c r="E170" s="15"/>
+      <c r="F170" s="15"/>
+      <c r="G170" s="15"/>
+      <c r="H170" s="15"/>
+      <c r="I170" s="15"/>
+      <c r="J170" s="15"/>
+      <c r="K170" s="15"/>
+      <c r="L170" s="15"/>
+      <c r="M170" s="15"/>
+      <c r="N170" s="15"/>
+      <c r="O170" s="15"/>
+      <c r="P170" s="15"/>
+      <c r="Q170" s="15"/>
+      <c r="R170" s="15"/>
+      <c r="S170" s="15"/>
+      <c r="T170" s="17"/>
+    </row>
+    <row r="171" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C171" s="18"/>
+      <c r="D171" s="19"/>
+      <c r="E171" s="19"/>
+      <c r="F171" s="19"/>
+      <c r="G171" s="19"/>
+      <c r="H171" s="19"/>
+      <c r="I171" s="19"/>
+      <c r="J171" s="19"/>
+      <c r="K171" s="19"/>
+      <c r="L171" s="19"/>
+      <c r="M171" s="19"/>
+      <c r="N171" s="19"/>
+      <c r="O171" s="19"/>
+      <c r="P171" s="19"/>
+      <c r="Q171" s="19"/>
+      <c r="R171" s="19"/>
+      <c r="S171" s="19"/>
+      <c r="T171" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SVM word2vec del and incorporated to SVM file
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA0B880-FEC5-4D34-A3F4-E64CB65E81EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A83CC0-536D-4E09-A762-8C31670A835C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -2050,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
   <dimension ref="B2:AP351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="49" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="B190" zoomScale="49" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H143" sqref="H143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
word2vec svm l2 reg
</commit_message>
<xml_diff>
--- a/TREC/Progress Summary.xlsx
+++ b/TREC/Progress Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB4B42-F0AF-43DF-944C-FCF30513E138}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA7B01-1B95-4D80-9348-A06B5C20E737}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -2317,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE1635E-9C38-43A7-A9DA-ED36E54400E4}">
   <dimension ref="B2:XFD369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="30" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" zoomScale="32" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11617,13 +11617,13 @@
         <v>0.76</v>
       </c>
       <c r="H31" s="223">
-        <v>0.65</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="I31" s="224">
-        <v>0.7</v>
+        <v>0.64</v>
       </c>
       <c r="J31" s="225">
-        <v>0.75</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="K31" s="208"/>
       <c r="L31" s="209"/>
@@ -11658,13 +11658,13 @@
         <v>0.84199999999999997</v>
       </c>
       <c r="H32" s="223">
-        <v>0.625</v>
+        <v>0.56659999999999999</v>
       </c>
       <c r="I32" s="224">
-        <v>0.58299999999999996</v>
+        <v>0.56659999999999999</v>
       </c>
       <c r="J32" s="225">
-        <v>0.67</v>
+        <v>0.58879999999999999</v>
       </c>
       <c r="K32" s="208"/>
       <c r="L32" s="209"/>
@@ -11700,9 +11700,15 @@
       <c r="G33" s="222">
         <v>0.75</v>
       </c>
-      <c r="H33" s="223"/>
-      <c r="I33" s="224"/>
-      <c r="J33" s="225"/>
+      <c r="H33" s="223">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="I33" s="224">
+        <v>0.6</v>
+      </c>
+      <c r="J33" s="225">
+        <v>0.59299999999999997</v>
+      </c>
       <c r="K33" s="208"/>
       <c r="L33" s="209"/>
       <c r="M33" s="210"/>
@@ -11735,9 +11741,15 @@
       <c r="G34" s="222">
         <v>1.4E-3</v>
       </c>
-      <c r="H34" s="223"/>
-      <c r="I34" s="224"/>
-      <c r="J34" s="225"/>
+      <c r="H34" s="223">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="I34" s="224">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J34" s="225">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="K34" s="208"/>
       <c r="L34" s="209"/>
       <c r="M34" s="210"/>
@@ -11770,9 +11782,15 @@
       <c r="G35" s="222">
         <v>0.875</v>
       </c>
-      <c r="H35" s="223"/>
-      <c r="I35" s="224"/>
-      <c r="J35" s="225"/>
+      <c r="H35" s="223">
+        <v>0.56659999999999999</v>
+      </c>
+      <c r="I35" s="224">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="J35" s="225">
+        <v>0.58799999999999997</v>
+      </c>
       <c r="K35" s="208"/>
       <c r="L35" s="209"/>
       <c r="M35" s="210"/>
@@ -11805,9 +11823,15 @@
       <c r="G36" s="222">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="H36" s="223"/>
-      <c r="I36" s="224"/>
-      <c r="J36" s="225"/>
+      <c r="H36" s="223">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="I36" s="224">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="J36" s="225">
+        <v>9.1000000000000004E-3</v>
+      </c>
       <c r="K36" s="208"/>
       <c r="L36" s="209"/>
       <c r="M36" s="210"/>
@@ -22069,7 +22093,7 @@
         <v>131</v>
       </c>
       <c r="U327" s="35">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="328" spans="3:21" ht="18.5" x14ac:dyDescent="0.45">
@@ -22612,7 +22636,7 @@
         <v>131</v>
       </c>
       <c r="U358" s="35">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="359" spans="3:21" ht="18.5" x14ac:dyDescent="0.45">

</xml_diff>